<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_outputs.xlsx
+++ b/Outputs/MonteCarlo_sim_outputs.xlsx
@@ -390,13 +390,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:26">
       <c r="A1">
         <v>0</v>
       </c>
@@ -409,204 +409,1194 @@
       <c r="D1">
         <v>3</v>
       </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3308430057939454</v>
+        <v>0.3308412651911598</v>
       </c>
       <c r="C2">
-        <v>0.3315278994243716</v>
+        <v>0.3306015090716298</v>
       </c>
       <c r="D2">
-        <v>0.330267589732521</v>
+        <v>0.3309861959862554</v>
+      </c>
+      <c r="E2">
+        <v>0.3310665084834603</v>
+      </c>
+      <c r="F2">
+        <v>0.3309148380140436</v>
+      </c>
+      <c r="G2">
+        <v>0.3299777386720321</v>
+      </c>
+      <c r="H2">
+        <v>0.3304683291789891</v>
+      </c>
+      <c r="I2">
+        <v>0.3303587264902083</v>
+      </c>
+      <c r="J2">
+        <v>0.3298405885476698</v>
+      </c>
+      <c r="K2">
+        <v>0.3288760956857318</v>
+      </c>
+      <c r="L2">
+        <v>0.3304708176209367</v>
+      </c>
+      <c r="M2">
+        <v>0.3311158162828593</v>
+      </c>
+      <c r="N2">
+        <v>0.3309580121952422</v>
+      </c>
+      <c r="O2">
+        <v>0.330420245114218</v>
+      </c>
+      <c r="P2">
+        <v>0.3324796649001385</v>
+      </c>
+      <c r="Q2">
+        <v>0.3314827890733741</v>
+      </c>
+      <c r="R2">
+        <v>0.3295894005618479</v>
+      </c>
+      <c r="S2">
+        <v>0.3297314342675339</v>
+      </c>
+      <c r="T2">
+        <v>0.3302479870032424</v>
+      </c>
+      <c r="U2">
+        <v>0.3290362228984869</v>
+      </c>
+      <c r="V2">
+        <v>0.3295373259145071</v>
+      </c>
+      <c r="W2">
+        <v>0.332210078067991</v>
+      </c>
+      <c r="X2">
+        <v>0.3306722870313438</v>
+      </c>
+      <c r="Y2">
+        <v>0.3329387850666813</v>
+      </c>
+      <c r="Z2">
+        <v>0.3304607792497125</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>37.57245311268169</v>
+        <v>37.6026856898841</v>
       </c>
       <c r="C3">
-        <v>37.52368104616776</v>
+        <v>37.61647844005643</v>
       </c>
       <c r="D3">
-        <v>37.65933160884434</v>
+        <v>37.58890884447254</v>
+      </c>
+      <c r="E3">
+        <v>37.56988860894939</v>
+      </c>
+      <c r="F3">
+        <v>37.60330376730666</v>
+      </c>
+      <c r="G3">
+        <v>37.69858334625117</v>
+      </c>
+      <c r="H3">
+        <v>37.64817359585678</v>
+      </c>
+      <c r="I3">
+        <v>37.65677766730263</v>
+      </c>
+      <c r="J3">
+        <v>37.70332415758563</v>
+      </c>
+      <c r="K3">
+        <v>37.83389380864907</v>
+      </c>
+      <c r="L3">
+        <v>37.66341506407589</v>
+      </c>
+      <c r="M3">
+        <v>37.55572584308062</v>
+      </c>
+      <c r="N3">
+        <v>37.61614342807627</v>
+      </c>
+      <c r="O3">
+        <v>37.65642342784001</v>
+      </c>
+      <c r="P3">
+        <v>37.40740100141932</v>
+      </c>
+      <c r="Q3">
+        <v>37.51412621091004</v>
+      </c>
+      <c r="R3">
+        <v>37.73611181844139</v>
+      </c>
+      <c r="S3">
+        <v>37.74654274644631</v>
+      </c>
+      <c r="T3">
+        <v>37.67963760623424</v>
+      </c>
+      <c r="U3">
+        <v>37.79441148108779</v>
+      </c>
+      <c r="V3">
+        <v>37.74262472480572</v>
+      </c>
+      <c r="W3">
+        <v>37.44261692403803</v>
+      </c>
+      <c r="X3">
+        <v>37.61930360776196</v>
+      </c>
+      <c r="Y3">
+        <v>37.35268883369273</v>
+      </c>
+      <c r="Z3">
+        <v>37.65953202269483</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>940.6860260760618</v>
+        <v>940.5727937886202</v>
       </c>
       <c r="C4">
-        <v>937.7862151242216</v>
+        <v>941.0967627647242</v>
       </c>
       <c r="D4">
-        <v>942.0001191384682</v>
+        <v>940.0588903616571</v>
+      </c>
+      <c r="E4">
+        <v>939.3498176226873</v>
+      </c>
+      <c r="F4">
+        <v>940.8187092430761</v>
+      </c>
+      <c r="G4">
+        <v>943.3031838701698</v>
+      </c>
+      <c r="H4">
+        <v>941.3131785593345</v>
+      </c>
+      <c r="I4">
+        <v>942.4624381235302</v>
+      </c>
+      <c r="J4">
+        <v>943.5657767940634</v>
+      </c>
+      <c r="K4">
+        <v>946.7209807123247</v>
+      </c>
+      <c r="L4">
+        <v>942.0828027590837</v>
+      </c>
+      <c r="M4">
+        <v>939.5676473625722</v>
+      </c>
+      <c r="N4">
+        <v>940.6548913733176</v>
+      </c>
+      <c r="O4">
+        <v>942.5680458017771</v>
+      </c>
+      <c r="P4">
+        <v>934.5611941664305</v>
+      </c>
+      <c r="Q4">
+        <v>938.4078402832247</v>
+      </c>
+      <c r="R4">
+        <v>944.0899298385709</v>
+      </c>
+      <c r="S4">
+        <v>944.291162093177</v>
+      </c>
+      <c r="T4">
+        <v>942.452134133113</v>
+      </c>
+      <c r="U4">
+        <v>945.9275649694421</v>
+      </c>
+      <c r="V4">
+        <v>944.5953133569601</v>
+      </c>
+      <c r="W4">
+        <v>935.8666442677602</v>
+      </c>
+      <c r="X4">
+        <v>940.805205188177</v>
+      </c>
+      <c r="Y4">
+        <v>933.3043729421065</v>
+      </c>
+      <c r="Z4">
+        <v>942.1425210668376</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>108.2715720221538</v>
+        <v>108.409323006963</v>
       </c>
       <c r="C5">
-        <v>108.0517371202193</v>
+        <v>108.2189832131974</v>
       </c>
       <c r="D5">
-        <v>108.3869709439199</v>
+        <v>108.2507577162262</v>
+      </c>
+      <c r="E5">
+        <v>108.2486099855835</v>
+      </c>
+      <c r="F5">
+        <v>108.2019922957576</v>
+      </c>
+      <c r="G5">
+        <v>108.5561930783004</v>
+      </c>
+      <c r="H5">
+        <v>108.1839083143492</v>
+      </c>
+      <c r="I5">
+        <v>108.3628416312944</v>
+      </c>
+      <c r="J5">
+        <v>108.5392646975983</v>
+      </c>
+      <c r="K5">
+        <v>108.9580543614782</v>
+      </c>
+      <c r="L5">
+        <v>108.3763949898037</v>
+      </c>
+      <c r="M5">
+        <v>108.1270905268422</v>
+      </c>
+      <c r="N5">
+        <v>108.2567504547843</v>
+      </c>
+      <c r="O5">
+        <v>108.3754798109938</v>
+      </c>
+      <c r="P5">
+        <v>107.5203756430313</v>
+      </c>
+      <c r="Q5">
+        <v>108.115198790508</v>
+      </c>
+      <c r="R5">
+        <v>108.5664911784511</v>
+      </c>
+      <c r="S5">
+        <v>108.5120699175729</v>
+      </c>
+      <c r="T5">
+        <v>108.4565186696584</v>
+      </c>
+      <c r="U5">
+        <v>108.8906794959638</v>
+      </c>
+      <c r="V5">
+        <v>108.7067556125616</v>
+      </c>
+      <c r="W5">
+        <v>107.6461431501121</v>
+      </c>
+      <c r="X5">
+        <v>108.2169610931006</v>
+      </c>
+      <c r="Y5">
+        <v>107.5065721900693</v>
+      </c>
+      <c r="Z5">
+        <v>108.3668385264612</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>52203.84692149153</v>
+        <v>52296.75973621262</v>
       </c>
       <c r="C6">
-        <v>51960.3600248947</v>
+        <v>52179.05698205717</v>
       </c>
       <c r="D6">
-        <v>52336.75980028456</v>
+        <v>52169.27261577638</v>
+      </c>
+      <c r="E6">
+        <v>52140.28071734324</v>
+      </c>
+      <c r="F6">
+        <v>52154.85402258941</v>
+      </c>
+      <c r="G6">
+        <v>52500.9257070702</v>
+      </c>
+      <c r="H6">
+        <v>52156.42609502432</v>
+      </c>
+      <c r="I6">
+        <v>52320.41797230429</v>
+      </c>
+      <c r="J6">
+        <v>52485.86826535755</v>
+      </c>
+      <c r="K6">
+        <v>52893.13030503585</v>
+      </c>
+      <c r="L6">
+        <v>52320.94633153323</v>
+      </c>
+      <c r="M6">
+        <v>52057.38922112674</v>
+      </c>
+      <c r="N6">
+        <v>52202.2595854464</v>
+      </c>
+      <c r="O6">
+        <v>52340.81226923713</v>
+      </c>
+      <c r="P6">
+        <v>51497.50386726287</v>
+      </c>
+      <c r="Q6">
+        <v>52013.58538541062</v>
+      </c>
+      <c r="R6">
+        <v>52528.25916037607</v>
+      </c>
+      <c r="S6">
+        <v>52494.83626242854</v>
+      </c>
+      <c r="T6">
+        <v>52395.73518963327</v>
+      </c>
+      <c r="U6">
+        <v>52808.65127637103</v>
+      </c>
+      <c r="V6">
+        <v>52645.73397207011</v>
+      </c>
+      <c r="W6">
+        <v>51621.61805214352</v>
+      </c>
+      <c r="X6">
+        <v>52181.64405059872</v>
+      </c>
+      <c r="Y6">
+        <v>51438.35248666591</v>
+      </c>
+      <c r="Z6">
+        <v>52317.98298710082</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2817.555696302155</v>
+        <v>2656.132682717412</v>
       </c>
       <c r="C7">
-        <v>2444.94224178322</v>
+        <v>3233.864289194662</v>
       </c>
       <c r="D7">
-        <v>2415.749185908342</v>
+        <v>2839.869339722895</v>
+      </c>
+      <c r="E7">
+        <v>3293.969765496182</v>
+      </c>
+      <c r="F7">
+        <v>3049.402213298834</v>
+      </c>
+      <c r="G7">
+        <v>1910.457099037971</v>
+      </c>
+      <c r="H7">
+        <v>3394.180384294353</v>
+      </c>
+      <c r="I7">
+        <v>2611.301287123919</v>
+      </c>
+      <c r="J7">
+        <v>2956.90719320303</v>
+      </c>
+      <c r="K7">
+        <v>1918.705343213926</v>
+      </c>
+      <c r="L7">
+        <v>3089.210718477125</v>
+      </c>
+      <c r="M7">
+        <v>3456.983834972973</v>
+      </c>
+      <c r="N7">
+        <v>1824.069264615599</v>
+      </c>
+      <c r="O7">
+        <v>2688.824415003176</v>
+      </c>
+      <c r="P7">
+        <v>2131.550610455245</v>
+      </c>
+      <c r="Q7">
+        <v>3110.138152476022</v>
+      </c>
+      <c r="R7">
+        <v>2282.430607154814</v>
+      </c>
+      <c r="S7">
+        <v>2638.004482991204</v>
+      </c>
+      <c r="T7">
+        <v>2860.196027545719</v>
+      </c>
+      <c r="U7">
+        <v>2777.75481292315</v>
+      </c>
+      <c r="V7">
+        <v>2166.388662879926</v>
+      </c>
+      <c r="W7">
+        <v>2678.496394011786</v>
+      </c>
+      <c r="X7">
+        <v>2331.465459679528</v>
+      </c>
+      <c r="Y7">
+        <v>2450.285630407299</v>
+      </c>
+      <c r="Z7">
+        <v>2970.505355546186</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2038.632092772528</v>
+        <v>1886.581615043594</v>
       </c>
       <c r="C8">
-        <v>2048.812036754298</v>
+        <v>1818.727832545421</v>
       </c>
       <c r="D8">
-        <v>1664.938583431613</v>
+        <v>1966.559332703682</v>
+      </c>
+      <c r="E8">
+        <v>1645.570490775785</v>
+      </c>
+      <c r="F8">
+        <v>2387.875238220753</v>
+      </c>
+      <c r="G8">
+        <v>1400.012280301944</v>
+      </c>
+      <c r="H8">
+        <v>2588.661478119214</v>
+      </c>
+      <c r="I8">
+        <v>3048.269757331725</v>
+      </c>
+      <c r="J8">
+        <v>1554.771063497869</v>
+      </c>
+      <c r="K8">
+        <v>1397.458947654269</v>
+      </c>
+      <c r="L8">
+        <v>1749.611080245301</v>
+      </c>
+      <c r="M8">
+        <v>2274.693908467363</v>
+      </c>
+      <c r="N8">
+        <v>1487.88547727646</v>
+      </c>
+      <c r="O8">
+        <v>1665.934863806598</v>
+      </c>
+      <c r="P8">
+        <v>768.6506045620273</v>
+      </c>
+      <c r="Q8">
+        <v>2164.163106586344</v>
+      </c>
+      <c r="R8">
+        <v>2160.861870249109</v>
+      </c>
+      <c r="S8">
+        <v>1837.195193452909</v>
+      </c>
+      <c r="T8">
+        <v>989.0254605814326</v>
+      </c>
+      <c r="U8">
+        <v>2160.421756679783</v>
+      </c>
+      <c r="V8">
+        <v>1550.175180571885</v>
+      </c>
+      <c r="W8">
+        <v>1059.522526290143</v>
+      </c>
+      <c r="X8">
+        <v>1530.776955797806</v>
+      </c>
+      <c r="Y8">
+        <v>1680.667937026263</v>
+      </c>
+      <c r="Z8">
+        <v>1935.07982633823</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>418.1121700421473</v>
+        <v>419.9061587117278</v>
       </c>
       <c r="C9">
-        <v>417.0320832440725</v>
+        <v>418.2455171409873</v>
       </c>
       <c r="D9">
-        <v>419.1212964195619</v>
+        <v>418.0645656545552</v>
+      </c>
+      <c r="E9">
+        <v>418.127070638816</v>
+      </c>
+      <c r="F9">
+        <v>418.100549856349</v>
+      </c>
+      <c r="G9">
+        <v>420.0999898903666</v>
+      </c>
+      <c r="H9">
+        <v>418.1428550176486</v>
+      </c>
+      <c r="I9">
+        <v>419.8613454937362</v>
+      </c>
+      <c r="J9">
+        <v>418.7358177005075</v>
+      </c>
+      <c r="K9">
+        <v>421.8618055164723</v>
+      </c>
+      <c r="L9">
+        <v>419.0736235182031</v>
+      </c>
+      <c r="M9">
+        <v>416.5030082944917</v>
+      </c>
+      <c r="N9">
+        <v>417.8143613463967</v>
+      </c>
+      <c r="O9">
+        <v>417.9021121679828</v>
+      </c>
+      <c r="P9">
+        <v>413.4573456048512</v>
+      </c>
+      <c r="Q9">
+        <v>416.560641698399</v>
+      </c>
+      <c r="R9">
+        <v>418.9964184641357</v>
+      </c>
+      <c r="S9">
+        <v>420.1351869995174</v>
+      </c>
+      <c r="T9">
+        <v>418.4844149633024</v>
+      </c>
+      <c r="U9">
+        <v>422.4362525153549</v>
+      </c>
+      <c r="V9">
+        <v>420.8135315613717</v>
+      </c>
+      <c r="W9">
+        <v>415.2475826862096</v>
+      </c>
+      <c r="X9">
+        <v>419.4263901776624</v>
+      </c>
+      <c r="Y9">
+        <v>413.2782999561436</v>
+      </c>
+      <c r="Z9">
+        <v>418.159472833941</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3337.840084422714</v>
+        <v>1891.009078142638</v>
       </c>
       <c r="C10">
-        <v>2123.808792864059</v>
+        <v>2812.775966966888</v>
       </c>
       <c r="D10">
-        <v>2744.28621137051</v>
+        <v>3138.889671599916</v>
+      </c>
+      <c r="E10">
+        <v>3085.781384228839</v>
+      </c>
+      <c r="F10">
+        <v>3256.382129012552</v>
+      </c>
+      <c r="G10">
+        <v>1434.861707168371</v>
+      </c>
+      <c r="H10">
+        <v>3162.219162610229</v>
+      </c>
+      <c r="I10">
+        <v>2760.960392570172</v>
+      </c>
+      <c r="J10">
+        <v>2226.312654457247</v>
+      </c>
+      <c r="K10">
+        <v>414.7847971533441</v>
+      </c>
+      <c r="L10">
+        <v>2366.107759080706</v>
+      </c>
+      <c r="M10">
+        <v>3511.036032320933</v>
+      </c>
+      <c r="N10">
+        <v>811.5911643498944</v>
+      </c>
+      <c r="O10">
+        <v>2710.913202051585</v>
+      </c>
+      <c r="P10">
+        <v>1778.133463471903</v>
+      </c>
+      <c r="Q10">
+        <v>3025.216951318089</v>
+      </c>
+      <c r="R10">
+        <v>1371.817236867345</v>
+      </c>
+      <c r="S10">
+        <v>2021.079976766879</v>
+      </c>
+      <c r="T10">
+        <v>2304.393017990417</v>
+      </c>
+      <c r="U10">
+        <v>2817.104265140621</v>
+      </c>
+      <c r="V10">
+        <v>2006.460378968996</v>
+      </c>
+      <c r="W10">
+        <v>2609.072841664622</v>
+      </c>
+      <c r="X10">
+        <v>2113.349044628165</v>
+      </c>
+      <c r="Y10">
+        <v>2430.630868150937</v>
+      </c>
+      <c r="Z10">
+        <v>2663.465697357442</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3537.89820132659</v>
+        <v>2533.656650032545</v>
       </c>
       <c r="C11">
-        <v>4395.098567625923</v>
+        <v>3107.580524319611</v>
       </c>
       <c r="D11">
-        <v>3364.393113022588</v>
+        <v>4402.933556309809</v>
+      </c>
+      <c r="E11">
+        <v>2799.335520496079</v>
+      </c>
+      <c r="F11">
+        <v>3173.138465677314</v>
+      </c>
+      <c r="G11">
+        <v>1996.210451085687</v>
+      </c>
+      <c r="H11">
+        <v>4474.308239013018</v>
+      </c>
+      <c r="I11">
+        <v>3710.813293601413</v>
+      </c>
+      <c r="J11">
+        <v>3017.127848500992</v>
+      </c>
+      <c r="K11">
+        <v>2667.274678115339</v>
+      </c>
+      <c r="L11">
+        <v>3010.576378127921</v>
+      </c>
+      <c r="M11">
+        <v>3257.996138954894</v>
+      </c>
+      <c r="N11">
+        <v>2013.267974719977</v>
+      </c>
+      <c r="O11">
+        <v>4057.310339229131</v>
+      </c>
+      <c r="P11">
+        <v>2009.872487146828</v>
+      </c>
+      <c r="Q11">
+        <v>4330.459096132106</v>
+      </c>
+      <c r="R11">
+        <v>3176.453557274619</v>
+      </c>
+      <c r="S11">
+        <v>2391.517425191952</v>
+      </c>
+      <c r="T11">
+        <v>3082.279044436781</v>
+      </c>
+      <c r="U11">
+        <v>3112.014855921025</v>
+      </c>
+      <c r="V11">
+        <v>2379.647870108894</v>
+      </c>
+      <c r="W11">
+        <v>1959.842319319543</v>
+      </c>
+      <c r="X11">
+        <v>2510.401415790135</v>
+      </c>
+      <c r="Y11">
+        <v>1554.401281719805</v>
+      </c>
+      <c r="Z11">
+        <v>3032.692712186258</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-71.88296147203194</v>
+        <v>-70.44915012786502</v>
       </c>
       <c r="C12">
-        <v>-71.14679087168878</v>
+        <v>-71.35261252349258</v>
       </c>
       <c r="D12">
-        <v>-71.66670849231727</v>
+        <v>-71.00141876693114</v>
+      </c>
+      <c r="E12">
+        <v>-70.98166407623695</v>
+      </c>
+      <c r="F12">
+        <v>-70.98078360012809</v>
+      </c>
+      <c r="G12">
+        <v>-71.83104218285803</v>
+      </c>
+      <c r="H12">
+        <v>-71.64965540420383</v>
+      </c>
+      <c r="I12">
+        <v>-70.63180498615938</v>
+      </c>
+      <c r="J12">
+        <v>-73.0177730966997</v>
+      </c>
+      <c r="K12">
+        <v>-71.40976854407828</v>
+      </c>
+      <c r="L12">
+        <v>-72.00690842096671</v>
+      </c>
+      <c r="M12">
+        <v>-71.9608855893959</v>
+      </c>
+      <c r="N12">
+        <v>-71.87879763910345</v>
+      </c>
+      <c r="O12">
+        <v>-72.36117547038461</v>
+      </c>
+      <c r="P12">
+        <v>-72.09370280679087</v>
+      </c>
+      <c r="Q12">
+        <v>-71.9130053918727</v>
+      </c>
+      <c r="R12">
+        <v>-72.26770570507676</v>
+      </c>
+      <c r="S12">
+        <v>-71.32456799083023</v>
+      </c>
+      <c r="T12">
+        <v>-71.99089093114381</v>
+      </c>
+      <c r="U12">
+        <v>-71.28365420791346</v>
+      </c>
+      <c r="V12">
+        <v>-71.69422762124864</v>
+      </c>
+      <c r="W12">
+        <v>-71.28498968335467</v>
+      </c>
+      <c r="X12">
+        <v>-70.96581800864448</v>
+      </c>
+      <c r="Y12">
+        <v>-72.08496338437872</v>
+      </c>
+      <c r="Z12">
+        <v>-71.3824226298528</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-1.843689837849373</v>
+        <v>-1.257005745167359</v>
       </c>
       <c r="C13">
-        <v>-1.658559319876139</v>
+        <v>-1.855601692281451</v>
       </c>
       <c r="D13">
-        <v>-1.454410208617671</v>
+        <v>-1.683717237645483</v>
+      </c>
+      <c r="E13">
+        <v>-1.38757098242071</v>
+      </c>
+      <c r="F13">
+        <v>-1.448689161593389</v>
+      </c>
+      <c r="G13">
+        <v>-1.880521366098384</v>
+      </c>
+      <c r="H13">
+        <v>-1.295256364956151</v>
+      </c>
+      <c r="I13">
+        <v>-1.925650905615572</v>
+      </c>
+      <c r="J13">
+        <v>-1.365441966625885</v>
+      </c>
+      <c r="K13">
+        <v>-1.525867057928487</v>
+      </c>
+      <c r="L13">
+        <v>-1.251492438420068</v>
+      </c>
+      <c r="M13">
+        <v>-1.64147701855603</v>
+      </c>
+      <c r="N13">
+        <v>-1.675014045638074</v>
+      </c>
+      <c r="O13">
+        <v>-1.603696062208469</v>
+      </c>
+      <c r="P13">
+        <v>-1.519768113646453</v>
+      </c>
+      <c r="Q13">
+        <v>-1.630483871100028</v>
+      </c>
+      <c r="R13">
+        <v>-1.426671414654785</v>
+      </c>
+      <c r="S13">
+        <v>-1.433978668822841</v>
+      </c>
+      <c r="T13">
+        <v>-1.777973795136062</v>
+      </c>
+      <c r="U13">
+        <v>-1.396689721268315</v>
+      </c>
+      <c r="V13">
+        <v>-1.439122734863524</v>
+      </c>
+      <c r="W13">
+        <v>-1.306713941380286</v>
+      </c>
+      <c r="X13">
+        <v>-1.48195655924569</v>
+      </c>
+      <c r="Y13">
+        <v>-1.52909287939533</v>
+      </c>
+      <c r="Z13">
+        <v>-1.583726461284705</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-1.79047152084141</v>
+        <v>-1.203423716573157</v>
       </c>
       <c r="C14">
-        <v>-1.604692930055543</v>
+        <v>-1.802463513210407</v>
       </c>
       <c r="D14">
-        <v>-1.40131271369712</v>
+        <v>-1.629990575625961</v>
+      </c>
+      <c r="E14">
+        <v>-1.333857061986953</v>
+      </c>
+      <c r="F14">
+        <v>-1.395214369638724</v>
+      </c>
+      <c r="G14">
+        <v>-1.827444450025567</v>
+      </c>
+      <c r="H14">
+        <v>-1.242045811187628</v>
+      </c>
+      <c r="I14">
+        <v>-1.872355175206602</v>
+      </c>
+      <c r="J14">
+        <v>-1.312583134252268</v>
+      </c>
+      <c r="K14">
+        <v>-1.473646003009299</v>
+      </c>
+      <c r="L14">
+        <v>-1.197888382601321</v>
+      </c>
+      <c r="M14">
+        <v>-1.587528016514103</v>
+      </c>
+      <c r="N14">
+        <v>-1.6214453007078</v>
+      </c>
+      <c r="O14">
+        <v>-1.55039698826265</v>
+      </c>
+      <c r="P14">
+        <v>-1.465753330154813</v>
+      </c>
+      <c r="Q14">
+        <v>-1.576894025272719</v>
+      </c>
+      <c r="R14">
+        <v>-1.373692198153029</v>
+      </c>
+      <c r="S14">
+        <v>-1.38110477518343</v>
+      </c>
+      <c r="T14">
+        <v>-1.724355944512783</v>
+      </c>
+      <c r="U14">
+        <v>-1.344257098147094</v>
+      </c>
+      <c r="V14">
+        <v>-1.386308030494818</v>
+      </c>
+      <c r="W14">
+        <v>-1.252626274188947</v>
+      </c>
+      <c r="X14">
+        <v>-1.428311333483989</v>
+      </c>
+      <c r="Y14">
+        <v>-1.47419755880807</v>
+      </c>
+      <c r="Z14">
+        <v>-1.530403078550919</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1.594413205794632</v>
+        <v>2.201486423589678</v>
       </c>
       <c r="C15">
-        <v>1.813549133467005</v>
+        <v>1.574973794896769</v>
       </c>
       <c r="D15">
-        <v>1.973345189828925</v>
+        <v>1.783215506105525</v>
+      </c>
+      <c r="E15">
+        <v>2.078750069218879</v>
+      </c>
+      <c r="F15">
+        <v>2.003312908637024</v>
+      </c>
+      <c r="G15">
+        <v>1.546980843380421</v>
+      </c>
+      <c r="H15">
+        <v>2.136774264199974</v>
+      </c>
+      <c r="I15">
+        <v>1.515355947032991</v>
+      </c>
+      <c r="J15">
+        <v>2.048064919698245</v>
+      </c>
+      <c r="K15">
+        <v>1.847525040126579</v>
+      </c>
+      <c r="L15">
+        <v>2.207891184797737</v>
+      </c>
+      <c r="M15">
+        <v>1.840757197090848</v>
+      </c>
+      <c r="N15">
+        <v>1.780385192898711</v>
+      </c>
+      <c r="O15">
+        <v>1.838773408051217</v>
+      </c>
+      <c r="P15">
+        <v>1.961686901815357</v>
+      </c>
+      <c r="Q15">
+        <v>1.828154534944304</v>
+      </c>
+      <c r="R15">
+        <v>1.994160851774725</v>
+      </c>
+      <c r="S15">
+        <v>1.979304909951606</v>
+      </c>
+      <c r="T15">
+        <v>1.683108777638719</v>
+      </c>
+      <c r="U15">
+        <v>1.990966767821371</v>
+      </c>
+      <c r="V15">
+        <v>1.973153507382018</v>
+      </c>
+      <c r="W15">
+        <v>2.180995996651032</v>
+      </c>
+      <c r="X15">
+        <v>1.979034169623174</v>
+      </c>
+      <c r="Y15">
+        <v>2.010267655661356</v>
+      </c>
+      <c r="Z15">
+        <v>1.858602902047705</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -617,6 +1607,72 @@
         <v>2</v>
       </c>
       <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16">
+        <v>2</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+      <c r="X16">
+        <v>2</v>
+      </c>
+      <c r="Y16">
+        <v>2</v>
+      </c>
+      <c r="Z16">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   MonteCarlo_Data_Analysis.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_outputs.xlsx
+++ b/Outputs/MonteCarlo_sim_outputs.xlsx
@@ -556,154 +556,154 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3997736438720151</v>
+        <v>0.3997681632664617</v>
       </c>
       <c r="C2">
-        <v>0.400527203270902</v>
+        <v>0.3990398361585493</v>
       </c>
       <c r="D2">
-        <v>0.4013046541192798</v>
+        <v>0.401320594346092</v>
       </c>
       <c r="E2">
-        <v>0.4021339246176995</v>
+        <v>0.4016310785892168</v>
       </c>
       <c r="F2">
-        <v>0.4002881182509422</v>
+        <v>0.4003301376820416</v>
       </c>
       <c r="G2">
-        <v>0.4006947573743632</v>
+        <v>0.3985733485271362</v>
       </c>
       <c r="H2">
-        <v>0.4029757193563845</v>
+        <v>0.4029269453753187</v>
       </c>
       <c r="I2">
-        <v>0.399620699780782</v>
+        <v>0.4003160804552042</v>
       </c>
       <c r="J2">
-        <v>0.4001138588788181</v>
+        <v>0.3992087782322077</v>
       </c>
       <c r="K2">
-        <v>0.3968968087547746</v>
+        <v>0.3976527722096476</v>
       </c>
       <c r="L2">
-        <v>0.4017330603741074</v>
+        <v>0.4019724184340551</v>
       </c>
       <c r="M2">
-        <v>0.3999214306446973</v>
+        <v>0.3985385696064084</v>
       </c>
       <c r="N2">
-        <v>0.399364307243099</v>
+        <v>0.4013156963311391</v>
       </c>
       <c r="O2">
-        <v>0.3993214288292873</v>
+        <v>0.4004949994781438</v>
       </c>
       <c r="P2">
-        <v>0.4009059354698425</v>
+        <v>0.4006998100023103</v>
       </c>
       <c r="Q2">
-        <v>0.3999133971525045</v>
+        <v>0.4007873649493239</v>
       </c>
       <c r="R2">
-        <v>0.4003626724922308</v>
+        <v>0.4011964984485152</v>
       </c>
       <c r="S2">
-        <v>0.400190457492628</v>
+        <v>0.4007154519143659</v>
       </c>
       <c r="T2">
-        <v>0.3995881764118711</v>
+        <v>0.4002618360818571</v>
       </c>
       <c r="U2">
-        <v>0.3983277056291084</v>
+        <v>0.4003240231858324</v>
       </c>
       <c r="V2">
-        <v>0.4002790842099006</v>
+        <v>0.4002958990043082</v>
       </c>
       <c r="W2">
-        <v>0.3989419819904452</v>
+        <v>0.4004941757396214</v>
       </c>
       <c r="X2">
-        <v>0.3985594121081408</v>
+        <v>0.3994373527381428</v>
       </c>
       <c r="Y2">
-        <v>0.3980780449274313</v>
+        <v>0.4016400069391086</v>
       </c>
       <c r="Z2">
-        <v>0.4027026206788352</v>
+        <v>0.3994496181816592</v>
       </c>
       <c r="AA2">
-        <v>0.3991977018327421</v>
+        <v>0.4018176905676845</v>
       </c>
       <c r="AB2">
-        <v>0.399574565559312</v>
+        <v>0.40197580556076</v>
       </c>
       <c r="AC2">
-        <v>0.3993355888720082</v>
+        <v>0.4009935258272847</v>
       </c>
       <c r="AD2">
-        <v>0.4001498789563499</v>
+        <v>0.399412258737431</v>
       </c>
       <c r="AE2">
-        <v>0.3998695859282363</v>
+        <v>0.4025015180640983</v>
       </c>
       <c r="AF2">
-        <v>0.400371642568257</v>
+        <v>0.4004985401819986</v>
       </c>
       <c r="AG2">
-        <v>0.3998037804031325</v>
+        <v>0.4007694694357846</v>
       </c>
       <c r="AH2">
-        <v>0.4007177595129156</v>
+        <v>0.3999832546904541</v>
       </c>
       <c r="AI2">
-        <v>0.3995889198269195</v>
+        <v>0.3998401304038109</v>
       </c>
       <c r="AJ2">
-        <v>0.3999498689270934</v>
+        <v>0.4015571512887065</v>
       </c>
       <c r="AK2">
-        <v>0.3997898743820484</v>
+        <v>0.4018407046228118</v>
       </c>
       <c r="AL2">
-        <v>0.4002834032300072</v>
+        <v>0.4007329627427911</v>
       </c>
       <c r="AM2">
-        <v>0.4009603893243477</v>
+        <v>0.4006595095026207</v>
       </c>
       <c r="AN2">
-        <v>0.4021806855543682</v>
+        <v>0.3996490165195178</v>
       </c>
       <c r="AO2">
-        <v>0.3997629142955786</v>
+        <v>0.4020342381845691</v>
       </c>
       <c r="AP2">
-        <v>0.3991076206268613</v>
+        <v>0.4008580369191942</v>
       </c>
       <c r="AQ2">
-        <v>0.4007828161640164</v>
+        <v>0.4032862991392991</v>
       </c>
       <c r="AR2">
-        <v>0.3989380614631488</v>
+        <v>0.401449659691266</v>
       </c>
       <c r="AS2">
-        <v>0.4006530473052028</v>
+        <v>0.4012923542057555</v>
       </c>
       <c r="AT2">
-        <v>0.3998012963896012</v>
+        <v>0.3998066569327786</v>
       </c>
       <c r="AU2">
-        <v>0.399282492704188</v>
+        <v>0.4007748595929808</v>
       </c>
       <c r="AV2">
-        <v>0.3995821506066812</v>
+        <v>0.4001519297113355</v>
       </c>
       <c r="AW2">
-        <v>0.4016051325468625</v>
+        <v>0.3993616267075699</v>
       </c>
       <c r="AX2">
-        <v>0.3986378523073276</v>
+        <v>0.4013808636125741</v>
       </c>
       <c r="AY2">
-        <v>0.3999389658704248</v>
+        <v>0.4009352206726522</v>
       </c>
     </row>
     <row r="3" spans="1:51">
@@ -711,154 +711,154 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>45.7065481848006</v>
+        <v>45.69785175791824</v>
       </c>
       <c r="C3">
-        <v>45.61835961123032</v>
+        <v>45.79220258686634</v>
       </c>
       <c r="D3">
-        <v>45.51512420667399</v>
+        <v>45.53483683755868</v>
       </c>
       <c r="E3">
-        <v>45.43952098256745</v>
+        <v>45.49286693701295</v>
       </c>
       <c r="F3">
-        <v>45.63604211516777</v>
+        <v>45.63454078664126</v>
       </c>
       <c r="G3">
-        <v>45.60016643010231</v>
+        <v>45.83118069889461</v>
       </c>
       <c r="H3">
-        <v>45.3455952874245</v>
+        <v>45.34836832850005</v>
       </c>
       <c r="I3">
-        <v>45.71467465964808</v>
+        <v>45.62613773892337</v>
       </c>
       <c r="J3">
-        <v>45.64889363440917</v>
+        <v>45.77019348751303</v>
       </c>
       <c r="K3">
-        <v>46.01385116689558</v>
+        <v>45.92166398930443</v>
       </c>
       <c r="L3">
-        <v>45.47268572568815</v>
+        <v>45.43484577642661</v>
       </c>
       <c r="M3">
-        <v>45.67509096737753</v>
+        <v>45.85576736511476</v>
       </c>
       <c r="N3">
-        <v>45.736990165751</v>
+        <v>45.52755220009698</v>
       </c>
       <c r="O3">
-        <v>45.74939228838473</v>
+        <v>45.63183159957971</v>
       </c>
       <c r="P3">
-        <v>45.56855447703256</v>
+        <v>45.59309236436332</v>
       </c>
       <c r="Q3">
-        <v>45.67533115606022</v>
+        <v>45.57382515930296</v>
       </c>
       <c r="R3">
-        <v>45.62719078043831</v>
+        <v>45.54536645415567</v>
       </c>
       <c r="S3">
-        <v>45.64884070894976</v>
+        <v>45.59190721477853</v>
       </c>
       <c r="T3">
-        <v>45.73771392139896</v>
+        <v>45.64447437861433</v>
       </c>
       <c r="U3">
-        <v>45.87010129312485</v>
+        <v>45.63856063439881</v>
       </c>
       <c r="V3">
-        <v>45.6327040811606</v>
+        <v>45.61742694979373</v>
       </c>
       <c r="W3">
-        <v>45.79790211058739</v>
+        <v>45.59545951988775</v>
       </c>
       <c r="X3">
-        <v>45.85948697092804</v>
+        <v>45.73965937186503</v>
       </c>
       <c r="Y3">
-        <v>45.89969617065015</v>
+        <v>45.47516105404524</v>
       </c>
       <c r="Z3">
-        <v>45.35647267806691</v>
+        <v>45.72766321694987</v>
       </c>
       <c r="AA3">
-        <v>45.77631537359521</v>
+        <v>45.46042266380896</v>
       </c>
       <c r="AB3">
-        <v>45.72681206103308</v>
+        <v>45.43143168234805</v>
       </c>
       <c r="AC3">
-        <v>45.74011647532404</v>
+        <v>45.54754080136749</v>
       </c>
       <c r="AD3">
-        <v>45.67030645810556</v>
+        <v>45.7389138920064</v>
       </c>
       <c r="AE3">
-        <v>45.68848097946088</v>
+        <v>45.38519847504638</v>
       </c>
       <c r="AF3">
-        <v>45.62278200399961</v>
+        <v>45.61702653212352</v>
       </c>
       <c r="AG3">
-        <v>45.68785989866125</v>
+        <v>45.58278287124937</v>
       </c>
       <c r="AH3">
-        <v>45.60540305693095</v>
+        <v>45.67838365039405</v>
       </c>
       <c r="AI3">
-        <v>45.7216993200794</v>
+        <v>45.6795871464146</v>
       </c>
       <c r="AJ3">
-        <v>45.67252836736115</v>
+        <v>45.48473502567857</v>
       </c>
       <c r="AK3">
-        <v>45.6929002806373</v>
+        <v>45.46917367823628</v>
       </c>
       <c r="AL3">
-        <v>45.6457303764998</v>
+        <v>45.59598461502637</v>
       </c>
       <c r="AM3">
-        <v>45.57339536849634</v>
+        <v>45.61099020083078</v>
       </c>
       <c r="AN3">
-        <v>45.4161182029275</v>
+        <v>45.72150291195745</v>
       </c>
       <c r="AO3">
-        <v>45.69024789176268</v>
+        <v>45.43523052087007</v>
       </c>
       <c r="AP3">
-        <v>45.77316968149992</v>
+        <v>45.59147444337523</v>
       </c>
       <c r="AQ3">
-        <v>45.58793767731374</v>
+        <v>45.27840321616535</v>
       </c>
       <c r="AR3">
-        <v>45.7805663469611</v>
+        <v>45.5006606036694</v>
       </c>
       <c r="AS3">
-        <v>45.6034015117134</v>
+        <v>45.54215997921171</v>
       </c>
       <c r="AT3">
-        <v>45.68378486678625</v>
+        <v>45.69665643679593</v>
       </c>
       <c r="AU3">
-        <v>45.75252423993985</v>
+        <v>45.56401322403597</v>
       </c>
       <c r="AV3">
-        <v>45.71990804009798</v>
+        <v>45.6352254326244</v>
       </c>
       <c r="AW3">
-        <v>45.48470797172341</v>
+        <v>45.73311398200666</v>
       </c>
       <c r="AX3">
-        <v>45.84198744320096</v>
+        <v>45.50544337052145</v>
       </c>
       <c r="AY3">
-        <v>45.67898350139988</v>
+        <v>45.56814196382792</v>
       </c>
     </row>
     <row r="4" spans="1:51">
@@ -866,154 +866,154 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>746.8700085539622</v>
+        <v>734.267202510995</v>
       </c>
       <c r="C4">
-        <v>730.2051025738714</v>
+        <v>745.9028200090271</v>
       </c>
       <c r="D4">
-        <v>728.0771504636235</v>
+        <v>728.0932875827946</v>
       </c>
       <c r="E4">
-        <v>736.4879374779607</v>
+        <v>727.4572301772546</v>
       </c>
       <c r="F4">
-        <v>727.3790440094682</v>
+        <v>724.7291403235662</v>
       </c>
       <c r="G4">
-        <v>755.0103055348854</v>
+        <v>762.6663072211937</v>
       </c>
       <c r="H4">
-        <v>716.0034514245709</v>
+        <v>758.4473607987568</v>
       </c>
       <c r="I4">
-        <v>753.9720145013591</v>
+        <v>739.7294240168673</v>
       </c>
       <c r="J4">
-        <v>762.4246528658</v>
+        <v>752.0679729846862</v>
       </c>
       <c r="K4">
-        <v>750.0308628899855</v>
+        <v>729.5122004974166</v>
       </c>
       <c r="L4">
-        <v>726.985624554966</v>
+        <v>729.6485176346953</v>
       </c>
       <c r="M4">
-        <v>744.6763339580513</v>
+        <v>730.3561559745881</v>
       </c>
       <c r="N4">
-        <v>738.614489925727</v>
+        <v>758.638235019258</v>
       </c>
       <c r="O4">
-        <v>714.3080609523315</v>
+        <v>759.8519552684195</v>
       </c>
       <c r="P4">
-        <v>731.6616788755156</v>
+        <v>724.6716878609475</v>
       </c>
       <c r="Q4">
-        <v>753.2948581040038</v>
+        <v>723.7451299362909</v>
       </c>
       <c r="R4">
-        <v>731.082159645364</v>
+        <v>763.0447320488346</v>
       </c>
       <c r="S4">
-        <v>759.107785832799</v>
+        <v>747.1640963799762</v>
       </c>
       <c r="T4">
-        <v>729.0527906410722</v>
+        <v>746.4926066353148</v>
       </c>
       <c r="U4">
-        <v>723.9433737427585</v>
+        <v>745.3442279616927</v>
       </c>
       <c r="V4">
-        <v>736.5595048981231</v>
+        <v>758.4874704548308</v>
       </c>
       <c r="W4">
-        <v>745.3797540453811</v>
+        <v>739.5911984078513</v>
       </c>
       <c r="X4">
-        <v>732.6244247657191</v>
+        <v>712.2615074444694</v>
       </c>
       <c r="Y4">
-        <v>734.708803160077</v>
+        <v>736.165166245827</v>
       </c>
       <c r="Z4">
-        <v>719.624896193734</v>
+        <v>743.6665129437433</v>
       </c>
       <c r="AA4">
-        <v>738.3602729082912</v>
+        <v>768.3178147501216</v>
       </c>
       <c r="AB4">
-        <v>731.2952161426457</v>
+        <v>750.6036795617931</v>
       </c>
       <c r="AC4">
-        <v>739.5346206525041</v>
+        <v>736.9211160763987</v>
       </c>
       <c r="AD4">
-        <v>743.867216898029</v>
+        <v>739.3536624841628</v>
       </c>
       <c r="AE4">
-        <v>736.2324042094554</v>
+        <v>749.6440066561879</v>
       </c>
       <c r="AF4">
-        <v>741.0675200145059</v>
+        <v>739.1341242833714</v>
       </c>
       <c r="AG4">
-        <v>745.5920573535352</v>
+        <v>733.5508738581678</v>
       </c>
       <c r="AH4">
-        <v>749.3881883336487</v>
+        <v>741.5619551923177</v>
       </c>
       <c r="AI4">
-        <v>745.968138533359</v>
+        <v>742.1483383607829</v>
       </c>
       <c r="AJ4">
-        <v>708.332229987391</v>
+        <v>716.5304788820665</v>
       </c>
       <c r="AK4">
-        <v>733.8794642774724</v>
+        <v>749.8318208710548</v>
       </c>
       <c r="AL4">
-        <v>737.9297296373699</v>
+        <v>738.9964925470717</v>
       </c>
       <c r="AM4">
-        <v>732.0452658003271</v>
+        <v>744.2271908002544</v>
       </c>
       <c r="AN4">
-        <v>732.1870728090614</v>
+        <v>753.1283165106221</v>
       </c>
       <c r="AO4">
-        <v>742.942635959518</v>
+        <v>732.3955294678467</v>
       </c>
       <c r="AP4">
-        <v>745.5695299332866</v>
+        <v>734.6324342878652</v>
       </c>
       <c r="AQ4">
-        <v>743.767142787582</v>
+        <v>721.1236601770559</v>
       </c>
       <c r="AR4">
-        <v>729.9701382039281</v>
+        <v>750.5857822176339</v>
       </c>
       <c r="AS4">
-        <v>764.7171503902835</v>
+        <v>768.0094159785179</v>
       </c>
       <c r="AT4">
-        <v>745.6022642383732</v>
+        <v>750.1097607767699</v>
       </c>
       <c r="AU4">
-        <v>737.7586803674683</v>
+        <v>736.5427717066934</v>
       </c>
       <c r="AV4">
-        <v>734.7790666798585</v>
+        <v>735.2483794690023</v>
       </c>
       <c r="AW4">
-        <v>744.5988671810826</v>
+        <v>744.9800997078762</v>
       </c>
       <c r="AX4">
-        <v>741.4473568056681</v>
+        <v>735.4577884527963</v>
       </c>
       <c r="AY4">
-        <v>735.7307871032465</v>
+        <v>751.287470634085</v>
       </c>
     </row>
     <row r="5" spans="1:51">
@@ -1021,154 +1021,154 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>69.2100011014259</v>
+        <v>68.56295880359258</v>
       </c>
       <c r="C5">
-        <v>69.02925255261403</v>
+        <v>69.88642257162026</v>
       </c>
       <c r="D5">
-        <v>68.79876469191119</v>
+        <v>67.72651687358578</v>
       </c>
       <c r="E5">
-        <v>69.00763309457157</v>
+        <v>68.91686918652462</v>
       </c>
       <c r="F5">
-        <v>65.55690556799156</v>
+        <v>68.3391054590101</v>
       </c>
       <c r="G5">
-        <v>70.88336517636732</v>
+        <v>72.02594881444787</v>
       </c>
       <c r="H5">
-        <v>67.34520028265223</v>
+        <v>69.01681388946719</v>
       </c>
       <c r="I5">
-        <v>69.43051147078776</v>
+        <v>68.87033254089397</v>
       </c>
       <c r="J5">
-        <v>71.78256421905967</v>
+        <v>70.94841548526757</v>
       </c>
       <c r="K5">
-        <v>71.92890649372599</v>
+        <v>67.94351389208482</v>
       </c>
       <c r="L5">
-        <v>69.49788609791173</v>
+        <v>67.11890641177693</v>
       </c>
       <c r="M5">
-        <v>68.94639901534828</v>
+        <v>67.71356315273167</v>
       </c>
       <c r="N5">
-        <v>69.29612836222223</v>
+        <v>71.50950006450816</v>
       </c>
       <c r="O5">
-        <v>66.96675762187705</v>
+        <v>71.52689546525299</v>
       </c>
       <c r="P5">
-        <v>69.09116646266996</v>
+        <v>67.69725318809276</v>
       </c>
       <c r="Q5">
-        <v>70.40441872134035</v>
+        <v>66.13664573522991</v>
       </c>
       <c r="R5">
-        <v>66.89602086836528</v>
+        <v>71.56357554937782</v>
       </c>
       <c r="S5">
-        <v>70.21775549248886</v>
+        <v>69.91526941670013</v>
       </c>
       <c r="T5">
-        <v>69.44665975115763</v>
+        <v>69.47248034289757</v>
       </c>
       <c r="U5">
-        <v>67.31643077172049</v>
+        <v>69.89432896291407</v>
       </c>
       <c r="V5">
-        <v>68.53336742524873</v>
+        <v>73.14500363786398</v>
       </c>
       <c r="W5">
-        <v>69.42147407319109</v>
+        <v>70.41339919586115</v>
       </c>
       <c r="X5">
-        <v>67.16162965580502</v>
+        <v>65.86460958967565</v>
       </c>
       <c r="Y5">
-        <v>68.13332572965925</v>
+        <v>66.45633425412242</v>
       </c>
       <c r="Z5">
-        <v>68.69985740257501</v>
+        <v>70.27588513406859</v>
       </c>
       <c r="AA5">
-        <v>68.2583898253385</v>
+        <v>73.2866541470021</v>
       </c>
       <c r="AB5">
-        <v>67.66661189187658</v>
+        <v>70.89858944729031</v>
       </c>
       <c r="AC5">
-        <v>69.86283409617427</v>
+        <v>70.73875796857382</v>
       </c>
       <c r="AD5">
-        <v>71.4825355534155</v>
+        <v>70.88872357049864</v>
       </c>
       <c r="AE5">
-        <v>70.05519593088003</v>
+        <v>72.01234241067468</v>
       </c>
       <c r="AF5">
-        <v>69.31058115709921</v>
+        <v>68.55400050820126</v>
       </c>
       <c r="AG5">
-        <v>69.28407296816961</v>
+        <v>67.95537929588845</v>
       </c>
       <c r="AH5">
-        <v>70.69665777294283</v>
+        <v>69.94963825698311</v>
       </c>
       <c r="AI5">
-        <v>70.7444418532275</v>
+        <v>68.31851873005601</v>
       </c>
       <c r="AJ5">
-        <v>65.3064132137746</v>
+        <v>65.25409499201383</v>
       </c>
       <c r="AK5">
-        <v>69.71927619847119</v>
+        <v>70.75914849354591</v>
       </c>
       <c r="AL5">
-        <v>70.37286318174917</v>
+        <v>69.63281041041108</v>
       </c>
       <c r="AM5">
-        <v>68.03480844587862</v>
+        <v>70.61415794015882</v>
       </c>
       <c r="AN5">
-        <v>68.61504959838122</v>
+        <v>71.64255741450617</v>
       </c>
       <c r="AO5">
-        <v>69.11329792226449</v>
+        <v>68.80444502776687</v>
       </c>
       <c r="AP5">
-        <v>67.47929808031523</v>
+        <v>69.26450916393793</v>
       </c>
       <c r="AQ5">
-        <v>70.13649179367847</v>
+        <v>66.46018910492272</v>
       </c>
       <c r="AR5">
-        <v>67.21409058183825</v>
+        <v>70.00201265262292</v>
       </c>
       <c r="AS5">
-        <v>72.38063721005453</v>
+        <v>73.15695263380043</v>
       </c>
       <c r="AT5">
-        <v>70.46784531376117</v>
+        <v>69.5324671534916</v>
       </c>
       <c r="AU5">
-        <v>68.50985912548025</v>
+        <v>68.36562573095834</v>
       </c>
       <c r="AV5">
-        <v>68.85010144934257</v>
+        <v>67.6993412128349</v>
       </c>
       <c r="AW5">
-        <v>70.14423012336877</v>
+        <v>69.49901579634924</v>
       </c>
       <c r="AX5">
-        <v>68.8764540585709</v>
+        <v>71.44049503213405</v>
       </c>
       <c r="AY5">
-        <v>66.80511611811673</v>
+        <v>71.13658014233792</v>
       </c>
     </row>
     <row r="6" spans="1:51">
@@ -1176,154 +1176,154 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>23737.94252143071</v>
+        <v>23219.92432860866</v>
       </c>
       <c r="C6">
-        <v>23414.45665967162</v>
+        <v>24062.94128893156</v>
       </c>
       <c r="D6">
-        <v>23219.29687742967</v>
+        <v>22741.1880106502</v>
       </c>
       <c r="E6">
-        <v>23402.14199715085</v>
+        <v>23262.34714517966</v>
       </c>
       <c r="F6">
-        <v>21645.05299137222</v>
+        <v>22994.66177910367</v>
       </c>
       <c r="G6">
-        <v>24673.48813990307</v>
+        <v>25325.94604372123</v>
       </c>
       <c r="H6">
-        <v>22391.02441935431</v>
+        <v>23731.97791524638</v>
       </c>
       <c r="I6">
-        <v>23908.20611991394</v>
+        <v>23453.26598867555</v>
       </c>
       <c r="J6">
-        <v>25242.20522129847</v>
+        <v>24693.88258145766</v>
       </c>
       <c r="K6">
-        <v>25185.01436458277</v>
+        <v>22875.90523637355</v>
       </c>
       <c r="L6">
-        <v>23578.57928907308</v>
+        <v>22448.6951619069</v>
       </c>
       <c r="M6">
-        <v>23573.73056209397</v>
+        <v>22781.57630072234</v>
       </c>
       <c r="N6">
-        <v>23657.57600491293</v>
+        <v>25044.25648002033</v>
       </c>
       <c r="O6">
-        <v>22185.75290735175</v>
+        <v>25055.35462201678</v>
       </c>
       <c r="P6">
-        <v>23445.54991427575</v>
+        <v>22648.06385631854</v>
       </c>
       <c r="Q6">
-        <v>24382.07366283254</v>
+        <v>21900.30171413884</v>
       </c>
       <c r="R6">
-        <v>22392.70794208128</v>
+        <v>25107.63893276777</v>
       </c>
       <c r="S6">
-        <v>24334.73649919069</v>
+        <v>24047.04150317766</v>
       </c>
       <c r="T6">
-        <v>23599.16877493485</v>
+        <v>23840.99343440865</v>
       </c>
       <c r="U6">
-        <v>22491.94307837607</v>
+        <v>24046.52932687069</v>
       </c>
       <c r="V6">
-        <v>23231.39775713995</v>
+        <v>25868.72275801285</v>
       </c>
       <c r="W6">
-        <v>23808.90824435413</v>
+        <v>24229.06982182992</v>
       </c>
       <c r="X6">
-        <v>22513.35116223575</v>
+        <v>21628.07491012688</v>
       </c>
       <c r="Y6">
-        <v>23033.57128464053</v>
+        <v>22163.29710341417</v>
       </c>
       <c r="Z6">
-        <v>23084.02474805331</v>
+        <v>24221.50003323627</v>
       </c>
       <c r="AA6">
-        <v>23137.65883088292</v>
+        <v>26099.51675613422</v>
       </c>
       <c r="AB6">
-        <v>22780.53190036974</v>
+        <v>24581.62495300042</v>
       </c>
       <c r="AC6">
-        <v>23945.03580080837</v>
+        <v>24330.5149228011</v>
       </c>
       <c r="AD6">
-        <v>24832.54158493362</v>
+        <v>24468.44289383654</v>
       </c>
       <c r="AE6">
-        <v>23969.46402052434</v>
+        <v>25155.85686167594</v>
       </c>
       <c r="AF6">
-        <v>23691.22030089336</v>
+        <v>23292.53841446832</v>
       </c>
       <c r="AG6">
-        <v>23721.92467436903</v>
+        <v>22906.76371792529</v>
       </c>
       <c r="AH6">
-        <v>24505.83466231401</v>
+        <v>23993.62050804364</v>
       </c>
       <c r="AI6">
-        <v>24496.48691511837</v>
+        <v>23203.75922911748</v>
       </c>
       <c r="AJ6">
-        <v>21317.18304096779</v>
+        <v>21356.66146499708</v>
       </c>
       <c r="AK6">
-        <v>23802.56353230551</v>
+        <v>24546.85638858539</v>
       </c>
       <c r="AL6">
-        <v>24156.98981538684</v>
+        <v>23834.40729313267</v>
       </c>
       <c r="AM6">
-        <v>22924.31201937038</v>
+        <v>24392.42532118483</v>
       </c>
       <c r="AN6">
-        <v>23212.99881020222</v>
+        <v>25065.25508678602</v>
       </c>
       <c r="AO6">
-        <v>23620.7964979871</v>
+        <v>23322.09686433966</v>
       </c>
       <c r="AP6">
-        <v>22820.71601842824</v>
+        <v>23599.27417474289</v>
       </c>
       <c r="AQ6">
-        <v>24132.32146052894</v>
+        <v>22019.02126734101</v>
       </c>
       <c r="AR6">
-        <v>22511.45529949858</v>
+        <v>24170.73583253819</v>
       </c>
       <c r="AS6">
-        <v>25562.93568663186</v>
+        <v>26035.02637646975</v>
       </c>
       <c r="AT6">
-        <v>24346.16683195245</v>
+        <v>23934.90975201841</v>
       </c>
       <c r="AU6">
-        <v>23261.89992857247</v>
+        <v>23171.40757714221</v>
       </c>
       <c r="AV6">
-        <v>23394.87676863619</v>
+        <v>22822.34338040895</v>
       </c>
       <c r="AW6">
-        <v>24160.87276964069</v>
+        <v>23868.22634481506</v>
       </c>
       <c r="AX6">
-        <v>23484.41966515925</v>
+        <v>24690.43104685203</v>
       </c>
       <c r="AY6">
-        <v>22348.9171306871</v>
+        <v>24739.25876757478</v>
       </c>
     </row>
     <row r="7" spans="1:51">
@@ -1331,154 +1331,154 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-897.9171512121281</v>
+        <v>-451.2195741735844</v>
       </c>
       <c r="C7">
-        <v>-443.937372716514</v>
+        <v>-478.8593172139538</v>
       </c>
       <c r="D7">
-        <v>-631.277685623627</v>
+        <v>-476.6773162224407</v>
       </c>
       <c r="E7">
-        <v>-678.7513691275891</v>
+        <v>-707.1255956060724</v>
       </c>
       <c r="F7">
-        <v>-726.8904091091911</v>
+        <v>-834.0357509705519</v>
       </c>
       <c r="G7">
-        <v>-301.7310730802428</v>
+        <v>-755.1161726431994</v>
       </c>
       <c r="H7">
-        <v>-184.6155516299254</v>
+        <v>-623.4435927695924</v>
       </c>
       <c r="I7">
-        <v>-695.7382189867316</v>
+        <v>-519.8410054170749</v>
       </c>
       <c r="J7">
-        <v>-1693.912563695625</v>
+        <v>-2196.99837921437</v>
       </c>
       <c r="K7">
-        <v>-730.5845334631032</v>
+        <v>-1203.166949153409</v>
       </c>
       <c r="L7">
-        <v>-251.2833567225728</v>
+        <v>-782.8618167200984</v>
       </c>
       <c r="M7">
-        <v>-583.082275288254</v>
+        <v>-973.3082644577614</v>
       </c>
       <c r="N7">
-        <v>-691.2078948548972</v>
+        <v>-659.5108260248774</v>
       </c>
       <c r="O7">
-        <v>-1357.385062576647</v>
+        <v>-1004.782427153561</v>
       </c>
       <c r="P7">
-        <v>-531.6576187432111</v>
+        <v>-895.8459421430541</v>
       </c>
       <c r="Q7">
-        <v>-916.803598064613</v>
+        <v>-1314.843370043732</v>
       </c>
       <c r="R7">
-        <v>-395.207795206238</v>
+        <v>-849.5385585594356</v>
       </c>
       <c r="S7">
-        <v>-844.2912186052653</v>
+        <v>-870.1352471520123</v>
       </c>
       <c r="T7">
-        <v>-876.6767412449803</v>
+        <v>-715.3591572954236</v>
       </c>
       <c r="U7">
-        <v>-1293.773916375303</v>
+        <v>-114.892019564896</v>
       </c>
       <c r="V7">
-        <v>-861.7821160099552</v>
+        <v>-327.270019358891</v>
       </c>
       <c r="W7">
-        <v>-838.2106806225753</v>
+        <v>-1349.335399460325</v>
       </c>
       <c r="X7">
-        <v>-1049.898278657316</v>
+        <v>-475.7905267152128</v>
       </c>
       <c r="Y7">
-        <v>-133.6651355835902</v>
+        <v>-191.3659380563113</v>
       </c>
       <c r="Z7">
-        <v>-957.1408967128995</v>
+        <v>-61.32615709088937</v>
       </c>
       <c r="AA7">
-        <v>-824.7157703288399</v>
+        <v>-859.3214007221492</v>
       </c>
       <c r="AB7">
-        <v>-442.5963463626029</v>
+        <v>-633.1350988618691</v>
       </c>
       <c r="AC7">
-        <v>-843.411431141932</v>
+        <v>-757.1717797437364</v>
       </c>
       <c r="AD7">
-        <v>-1191.199160466677</v>
+        <v>-98.04489449492333</v>
       </c>
       <c r="AE7">
-        <v>-670.6323947444946</v>
+        <v>-708.7283085410629</v>
       </c>
       <c r="AF7">
-        <v>-1170.842875862074</v>
+        <v>170.5502471173518</v>
       </c>
       <c r="AG7">
-        <v>-598.2265363725542</v>
+        <v>-744.6095129782954</v>
       </c>
       <c r="AH7">
-        <v>-1452.643431356333</v>
+        <v>-670.7756911856075</v>
       </c>
       <c r="AI7">
-        <v>-677.5711990856501</v>
+        <v>-1092.751816593206</v>
       </c>
       <c r="AJ7">
-        <v>-852.1839946464439</v>
+        <v>-136.1910863429886</v>
       </c>
       <c r="AK7">
-        <v>-890.8623114328666</v>
+        <v>-837.068759668064</v>
       </c>
       <c r="AL7">
-        <v>-523.3738019029706</v>
+        <v>-1174.052018765945</v>
       </c>
       <c r="AM7">
-        <v>-933.8840430774492</v>
+        <v>-636.7689734065452</v>
       </c>
       <c r="AN7">
-        <v>-472.3708840566468</v>
+        <v>-783.2385897833474</v>
       </c>
       <c r="AO7">
-        <v>-601.0224692765614</v>
+        <v>-429.5659816507055</v>
       </c>
       <c r="AP7">
-        <v>-287.9005979749799</v>
+        <v>-274.0044536605258</v>
       </c>
       <c r="AQ7">
-        <v>-813.778983078655</v>
+        <v>-857.7255886971849</v>
       </c>
       <c r="AR7">
-        <v>-1340.063318529335</v>
+        <v>-815.0675937263886</v>
       </c>
       <c r="AS7">
-        <v>-758.1538105664305</v>
+        <v>-1305.901384810972</v>
       </c>
       <c r="AT7">
-        <v>-561.3407334944259</v>
+        <v>-1026.184265071393</v>
       </c>
       <c r="AU7">
-        <v>-2580.073777551123</v>
+        <v>-740.2439429390645</v>
       </c>
       <c r="AV7">
-        <v>285.4301154710226</v>
+        <v>-902.0481007410942</v>
       </c>
       <c r="AW7">
-        <v>-370.4440435211037</v>
+        <v>-1173.32960427587</v>
       </c>
       <c r="AX7">
-        <v>-484.5762430131408</v>
+        <v>65.41695363936638</v>
       </c>
       <c r="AY7">
-        <v>-125.4293377714079</v>
+        <v>-923.3274432750349</v>
       </c>
     </row>
     <row r="8" spans="1:51">
@@ -1486,154 +1486,154 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-2403.678734546406</v>
+        <v>-2987.742936071878</v>
       </c>
       <c r="C8">
-        <v>-2913.766315384838</v>
+        <v>-3083.026003278774</v>
       </c>
       <c r="D8">
-        <v>-4248.004783071642</v>
+        <v>-2277.330439098938</v>
       </c>
       <c r="E8">
-        <v>-5470.17045681031</v>
+        <v>-4662.773614434371</v>
       </c>
       <c r="F8">
-        <v>-3615.531361814193</v>
+        <v>-2460.674923335289</v>
       </c>
       <c r="G8">
-        <v>-3199.041182597515</v>
+        <v>-4859.371992271717</v>
       </c>
       <c r="H8">
-        <v>-2339.243656151354</v>
+        <v>-3633.130265891502</v>
       </c>
       <c r="I8">
-        <v>-3112.585886870591</v>
+        <v>-2902.522969734132</v>
       </c>
       <c r="J8">
-        <v>-2384.443463879153</v>
+        <v>-636.9861711865169</v>
       </c>
       <c r="K8">
-        <v>-2739.034963916523</v>
+        <v>-2517.965510407162</v>
       </c>
       <c r="L8">
-        <v>-3146.200187629202</v>
+        <v>-3203.59694315398</v>
       </c>
       <c r="M8">
-        <v>-2707.413523897161</v>
+        <v>-2441.945245738953</v>
       </c>
       <c r="N8">
-        <v>-3442.009252958353</v>
+        <v>-2279.95710378224</v>
       </c>
       <c r="O8">
-        <v>1865.035120006937</v>
+        <v>-3740.153590838495</v>
       </c>
       <c r="P8">
-        <v>-3363.330802680524</v>
+        <v>-3612.957489414434</v>
       </c>
       <c r="Q8">
-        <v>-3967.705588293234</v>
+        <v>-2454.231425512226</v>
       </c>
       <c r="R8">
-        <v>-2434.96668550155</v>
+        <v>-3041.445923047888</v>
       </c>
       <c r="S8">
-        <v>-4327.242218878097</v>
+        <v>-4042.825706721031</v>
       </c>
       <c r="T8">
-        <v>-2882.319133798296</v>
+        <v>-3319.144301472688</v>
       </c>
       <c r="U8">
-        <v>-2859.09830850834</v>
+        <v>-2829.091510337144</v>
       </c>
       <c r="V8">
-        <v>-3475.136098661205</v>
+        <v>-4437.142449708047</v>
       </c>
       <c r="W8">
-        <v>-3211.726164349922</v>
+        <v>-2519.251583665654</v>
       </c>
       <c r="X8">
-        <v>-3417.091399994121</v>
+        <v>-2010.302723013668</v>
       </c>
       <c r="Y8">
-        <v>-3118.082878144278</v>
+        <v>-4891.533023333995</v>
       </c>
       <c r="Z8">
-        <v>-3053.976902300919</v>
+        <v>-2695.889389754378</v>
       </c>
       <c r="AA8">
-        <v>-2594.02596950735</v>
+        <v>-2311.198151821995</v>
       </c>
       <c r="AB8">
-        <v>-1889.06265198198</v>
+        <v>-4191.30904232985</v>
       </c>
       <c r="AC8">
-        <v>-3783.671372920501</v>
+        <v>-4361.405496781946</v>
       </c>
       <c r="AD8">
-        <v>-3336.101591878595</v>
+        <v>-3291.343806850083</v>
       </c>
       <c r="AE8">
-        <v>-4542.057939541765</v>
+        <v>-3961.51772330419</v>
       </c>
       <c r="AF8">
-        <v>-2940.685325798108</v>
+        <v>-2623.584776813545</v>
       </c>
       <c r="AG8">
-        <v>-3596.711943434126</v>
+        <v>-3150.654033302209</v>
       </c>
       <c r="AH8">
-        <v>-2891.480547150233</v>
+        <v>-4206.366759218756</v>
       </c>
       <c r="AI8">
-        <v>-2770.496293591286</v>
+        <v>-2774.725357430872</v>
       </c>
       <c r="AJ8">
-        <v>-2866.681597671839</v>
+        <v>-4361.896798251094</v>
       </c>
       <c r="AK8">
-        <v>-2985.735471606511</v>
+        <v>-2560.407064577046</v>
       </c>
       <c r="AL8">
-        <v>-4362.623782916443</v>
+        <v>-3179.815702571573</v>
       </c>
       <c r="AM8">
-        <v>-3970.269051915441</v>
+        <v>-2923.960379122002</v>
       </c>
       <c r="AN8">
-        <v>-3233.871663814444</v>
+        <v>-2111.511010563505</v>
       </c>
       <c r="AO8">
-        <v>-2337.168486704581</v>
+        <v>-2620.330704905567</v>
       </c>
       <c r="AP8">
-        <v>-2976.65556761565</v>
+        <v>-2397.485555733641</v>
       </c>
       <c r="AQ8">
-        <v>-3815.158609029791</v>
+        <v>-2454.262301000228</v>
       </c>
       <c r="AR8">
-        <v>-2197.638378406445</v>
+        <v>-2500.800076762891</v>
       </c>
       <c r="AS8">
-        <v>-3591.377479084157</v>
+        <v>-2073.095950318513</v>
       </c>
       <c r="AT8">
-        <v>-3114.938869353401</v>
+        <v>-2711.191139294556</v>
       </c>
       <c r="AU8">
-        <v>-313.1529162971117</v>
+        <v>-2187.348052770496</v>
       </c>
       <c r="AV8">
-        <v>-2778.032442896563</v>
+        <v>-2251.450865171273</v>
       </c>
       <c r="AW8">
-        <v>-2873.038832122238</v>
+        <v>-2079.441870948073</v>
       </c>
       <c r="AX8">
-        <v>-3321.826866382649</v>
+        <v>-3295.157581267806</v>
       </c>
       <c r="AY8">
-        <v>-3958.105078801838</v>
+        <v>-3717.402745411913</v>
       </c>
     </row>
     <row r="9" spans="1:51">
@@ -1641,154 +1641,154 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2193.50768038437</v>
+        <v>1970.453898125548</v>
       </c>
       <c r="C9">
-        <v>2187.291558327131</v>
+        <v>1986.94959784969</v>
       </c>
       <c r="D9">
-        <v>2187.992455063837</v>
+        <v>1952.365885128307</v>
       </c>
       <c r="E9">
-        <v>2186.156110658796</v>
+        <v>1969.528211907056</v>
       </c>
       <c r="F9">
-        <v>2133.021386323544</v>
+        <v>1970.269294442411</v>
       </c>
       <c r="G9">
-        <v>2216.83819003852</v>
+        <v>2022.383432035591</v>
       </c>
       <c r="H9">
-        <v>2160.50609606818</v>
+        <v>1983.065360195535</v>
       </c>
       <c r="I9">
-        <v>2202.565581029625</v>
+        <v>1974.71289885757</v>
       </c>
       <c r="J9">
-        <v>2232.09626978331</v>
+        <v>2010.382022420852</v>
       </c>
       <c r="K9">
-        <v>2235.708093817923</v>
+        <v>1956.902520849577</v>
       </c>
       <c r="L9">
-        <v>2194.089792329793</v>
+        <v>1943.763111136294</v>
       </c>
       <c r="M9">
-        <v>2185.012605247771</v>
+        <v>1955.532616194985</v>
       </c>
       <c r="N9">
-        <v>2191.830049032944</v>
+        <v>2025.374765000619</v>
       </c>
       <c r="O9">
-        <v>2158.528613439543</v>
+        <v>2018.073700929373</v>
       </c>
       <c r="P9">
-        <v>2193.484326511279</v>
+        <v>1959.912561702489</v>
       </c>
       <c r="Q9">
-        <v>2216.502139437288</v>
+        <v>1928.88087795875</v>
       </c>
       <c r="R9">
-        <v>2153.579084034649</v>
+        <v>2023.262627539888</v>
       </c>
       <c r="S9">
-        <v>2213.931763641436</v>
+        <v>1993.819600583708</v>
       </c>
       <c r="T9">
-        <v>2190.082012927979</v>
+        <v>1987.140033440613</v>
       </c>
       <c r="U9">
-        <v>2156.708715513174</v>
+        <v>1994.611617517267</v>
       </c>
       <c r="V9">
-        <v>2180.490425535565</v>
+        <v>2034.409408242823</v>
       </c>
       <c r="W9">
-        <v>2191.420965791589</v>
+        <v>2004.570866419581</v>
       </c>
       <c r="X9">
-        <v>2156.787626938386</v>
+        <v>1927.320179947979</v>
       </c>
       <c r="Y9">
-        <v>2176.912178341897</v>
+        <v>1932.739790125517</v>
       </c>
       <c r="Z9">
-        <v>2182.852313244158</v>
+        <v>2000.094040646851</v>
       </c>
       <c r="AA9">
-        <v>2180.005855409957</v>
+        <v>2039.670603816783</v>
       </c>
       <c r="AB9">
-        <v>2167.335961660266</v>
+        <v>2012.197760010869</v>
       </c>
       <c r="AC9">
-        <v>2203.716990282556</v>
+        <v>1996.986625620954</v>
       </c>
       <c r="AD9">
-        <v>2223.594790866963</v>
+        <v>2010.091149078162</v>
       </c>
       <c r="AE9">
-        <v>2204.098237399464</v>
+        <v>2017.57293120822</v>
       </c>
       <c r="AF9">
-        <v>2192.561256748347</v>
+        <v>1979.415398087764</v>
       </c>
       <c r="AG9">
-        <v>2199.312120234494</v>
+        <v>1958.261839535053</v>
       </c>
       <c r="AH9">
-        <v>2218.592602924006</v>
+        <v>1988.757203573333</v>
       </c>
       <c r="AI9">
-        <v>2215.60072451721</v>
+        <v>1969.365193220139</v>
       </c>
       <c r="AJ9">
-        <v>2116.236622968892</v>
+        <v>1921.498402562485</v>
       </c>
       <c r="AK9">
-        <v>2196.579059796306</v>
+        <v>2002.003547452109</v>
       </c>
       <c r="AL9">
-        <v>2211.263670859763</v>
+        <v>1979.098126046629</v>
       </c>
       <c r="AM9">
-        <v>2159.907688238864</v>
+        <v>2000.939985918805</v>
       </c>
       <c r="AN9">
-        <v>2182.820691051691</v>
+        <v>2017.179363685382</v>
       </c>
       <c r="AO9">
-        <v>2204.929888307442</v>
+        <v>1977.529454297649</v>
       </c>
       <c r="AP9">
-        <v>2176.515269633385</v>
+        <v>1979.131008020551</v>
       </c>
       <c r="AQ9">
-        <v>2194.941987069406</v>
+        <v>1929.551864509921</v>
       </c>
       <c r="AR9">
-        <v>2169.482654090983</v>
+        <v>1999.144724918634</v>
       </c>
       <c r="AS9">
-        <v>2241.809332193635</v>
+        <v>2039.302808198583</v>
       </c>
       <c r="AT9">
-        <v>2207.024088027365</v>
+        <v>1988.77267470061</v>
       </c>
       <c r="AU9">
-        <v>2184.287483118818</v>
+        <v>1965.738658357442</v>
       </c>
       <c r="AV9">
-        <v>2184.650836903374</v>
+        <v>1956.395575210298</v>
       </c>
       <c r="AW9">
-        <v>2204.574985508636</v>
+        <v>1989.898141264522</v>
       </c>
       <c r="AX9">
-        <v>2189.393365614309</v>
+        <v>2010.819276310717</v>
       </c>
       <c r="AY9">
-        <v>2158.613366573489</v>
+        <v>2004.800510035586</v>
       </c>
     </row>
     <row r="10" spans="1:51">
@@ -1796,154 +1796,154 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>7245.228862547246</v>
+        <v>11059.39210154268</v>
       </c>
       <c r="C10">
-        <v>12912.93771166012</v>
+        <v>14565.82924738614</v>
       </c>
       <c r="D10">
-        <v>11732.91837124656</v>
+        <v>14015.66792509672</v>
       </c>
       <c r="E10">
-        <v>18684.35407941887</v>
+        <v>17912.25093364022</v>
       </c>
       <c r="F10">
-        <v>11839.47971625057</v>
+        <v>8695.696746248148</v>
       </c>
       <c r="G10">
-        <v>17112.29352410834</v>
+        <v>14802.76004346149</v>
       </c>
       <c r="H10">
-        <v>16644.20957462862</v>
+        <v>10813.894333891</v>
       </c>
       <c r="I10">
-        <v>11766.72343845206</v>
+        <v>14067.13601322163</v>
       </c>
       <c r="J10">
-        <v>4319.384183087879</v>
+        <v>6768.373836691379</v>
       </c>
       <c r="K10">
-        <v>11694.94622123096</v>
+        <v>1356.113363364412</v>
       </c>
       <c r="L10">
-        <v>16166.3336369485</v>
+        <v>8550.901645890312</v>
       </c>
       <c r="M10">
-        <v>12381.14700637993</v>
+        <v>9597.60188525593</v>
       </c>
       <c r="N10">
-        <v>13170.823724433</v>
+        <v>14501.45388339004</v>
       </c>
       <c r="O10">
-        <v>8879.182414605664</v>
+        <v>13325.4549844001</v>
       </c>
       <c r="P10">
-        <v>15600.8822102845</v>
+        <v>12969.42519415856</v>
       </c>
       <c r="Q10">
-        <v>10426.08458399685</v>
+        <v>2960.375981381996</v>
       </c>
       <c r="R10">
-        <v>11207.07181671717</v>
+        <v>9325.823227052919</v>
       </c>
       <c r="S10">
-        <v>12534.66243809888</v>
+        <v>2806.074671943393</v>
       </c>
       <c r="T10">
-        <v>10858.47050372348</v>
+        <v>14206.53629088111</v>
       </c>
       <c r="U10">
-        <v>6597.514041797458</v>
+        <v>17445.15750701998</v>
       </c>
       <c r="V10">
-        <v>13472.95617329277</v>
+        <v>17571.78286142989</v>
       </c>
       <c r="W10">
-        <v>8211.497449605304</v>
+        <v>4082.114641685117</v>
       </c>
       <c r="X10">
-        <v>8831.292177421916</v>
+        <v>15257.19030763167</v>
       </c>
       <c r="Y10">
-        <v>17796.81837612602</v>
+        <v>15651.60630901766</v>
       </c>
       <c r="Z10">
-        <v>12956.84478725049</v>
+        <v>17970.82288424066</v>
       </c>
       <c r="AA10">
-        <v>15408.44880692224</v>
+        <v>7770.592927039062</v>
       </c>
       <c r="AB10">
-        <v>17349.12359052103</v>
+        <v>12879.56631339384</v>
       </c>
       <c r="AC10">
-        <v>6668.004081690657</v>
+        <v>11292.50052615689</v>
       </c>
       <c r="AD10">
-        <v>2721.170559719614</v>
+        <v>17777.885839328</v>
       </c>
       <c r="AE10">
-        <v>11891.19339549682</v>
+        <v>7283.957788173335</v>
       </c>
       <c r="AF10">
-        <v>3440.515091368925</v>
+        <v>18722.04412200813</v>
       </c>
       <c r="AG10">
-        <v>13590.3148003158</v>
+        <v>11101.74674018678</v>
       </c>
       <c r="AH10">
-        <v>3813.523072446305</v>
+        <v>12361.31770484394</v>
       </c>
       <c r="AI10">
-        <v>14188.23964190346</v>
+        <v>5544.264587345789</v>
       </c>
       <c r="AJ10">
-        <v>9890.866409551769</v>
+        <v>15909.71851094885</v>
       </c>
       <c r="AK10">
-        <v>6660.51214659343</v>
+        <v>8692.324780788083</v>
       </c>
       <c r="AL10">
-        <v>16321.37142388837</v>
+        <v>-468.7957553296237</v>
       </c>
       <c r="AM10">
-        <v>6974.515909582146</v>
+        <v>19506.82997819228</v>
       </c>
       <c r="AN10">
-        <v>8183.185011904823</v>
+        <v>9670.85377152462</v>
       </c>
       <c r="AO10">
-        <v>10279.60577990351</v>
+        <v>18721.84817563448</v>
       </c>
       <c r="AP10">
-        <v>11507.86658936772</v>
+        <v>19860.22369060457</v>
       </c>
       <c r="AQ10">
-        <v>7179.35879144623</v>
+        <v>8111.914215480521</v>
       </c>
       <c r="AR10">
-        <v>5511.753094889395</v>
+        <v>11358.29273121176</v>
       </c>
       <c r="AS10">
-        <v>8194.160140253594</v>
+        <v>7250.193193667528</v>
       </c>
       <c r="AT10">
-        <v>20060.93871365344</v>
+        <v>2683.042139626241</v>
       </c>
       <c r="AU10">
-        <v>10103.13280227273</v>
+        <v>7194.833765873264</v>
       </c>
       <c r="AV10">
-        <v>19609.96562107962</v>
+        <v>4617.652083368252</v>
       </c>
       <c r="AW10">
-        <v>20274.15211917985</v>
+        <v>-254.3876358903949</v>
       </c>
       <c r="AX10">
-        <v>14290.04087499226</v>
+        <v>18719.55574133428</v>
       </c>
       <c r="AY10">
-        <v>19896.02294988453</v>
+        <v>11048.42697585269</v>
       </c>
     </row>
     <row r="11" spans="1:51">
@@ -1951,154 +1951,154 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5892.549549368191</v>
+        <v>8565.731312151509</v>
       </c>
       <c r="C11">
-        <v>14839.77300114158</v>
+        <v>6144.838979657493</v>
       </c>
       <c r="D11">
-        <v>16626.41164036298</v>
+        <v>2614.520103675338</v>
       </c>
       <c r="E11">
-        <v>15529.12741148403</v>
+        <v>9163.80639849434</v>
       </c>
       <c r="F11">
-        <v>10535.07246773374</v>
+        <v>-3903.132122961318</v>
       </c>
       <c r="G11">
-        <v>10793.3282252873</v>
+        <v>13180.80332885616</v>
       </c>
       <c r="H11">
-        <v>-6093.077077825543</v>
+        <v>7829.773323354421</v>
       </c>
       <c r="I11">
-        <v>8853.118281793595</v>
+        <v>6159.081310736131</v>
       </c>
       <c r="J11">
-        <v>3039.634793346809</v>
+        <v>-3150.789727335775</v>
       </c>
       <c r="K11">
-        <v>677.6494313156693</v>
+        <v>1320.080094621209</v>
       </c>
       <c r="L11">
-        <v>4385.654729790843</v>
+        <v>10874.40169205812</v>
       </c>
       <c r="M11">
-        <v>2184.745387667264</v>
+        <v>5142.523518219173</v>
       </c>
       <c r="N11">
-        <v>6673.232017845683</v>
+        <v>-2462.92126676467</v>
       </c>
       <c r="O11">
-        <v>-9927.564032795461</v>
+        <v>5289.903112112217</v>
       </c>
       <c r="P11">
-        <v>3190.364699795356</v>
+        <v>15516.73061009363</v>
       </c>
       <c r="Q11">
-        <v>808.7476530521116</v>
+        <v>6453.305154158296</v>
       </c>
       <c r="R11">
-        <v>6868.20552140669</v>
+        <v>5495.200455572423</v>
       </c>
       <c r="S11">
-        <v>6434.630730850527</v>
+        <v>2837.947586345574</v>
       </c>
       <c r="T11">
-        <v>4372.764126844045</v>
+        <v>4390.378429854582</v>
       </c>
       <c r="U11">
-        <v>6839.918133065991</v>
+        <v>291.206186776081</v>
       </c>
       <c r="V11">
-        <v>13218.66738169194</v>
+        <v>-2512.596348135967</v>
       </c>
       <c r="W11">
-        <v>4125.959488624158</v>
+        <v>-2738.326014680736</v>
       </c>
       <c r="X11">
-        <v>4991.719753986195</v>
+        <v>6210.815411517444</v>
       </c>
       <c r="Y11">
-        <v>15738.5227296558</v>
+        <v>18403.32590650216</v>
       </c>
       <c r="Z11">
-        <v>10311.54802188635</v>
+        <v>1681.919578306704</v>
       </c>
       <c r="AA11">
-        <v>1529.159866500961</v>
+        <v>-584.7162379923184</v>
       </c>
       <c r="AB11">
-        <v>3299.216388001981</v>
+        <v>-474.1500734682867</v>
       </c>
       <c r="AC11">
-        <v>4949.212807766057</v>
+        <v>12103.1523745005</v>
       </c>
       <c r="AD11">
-        <v>4715.515803786684</v>
+        <v>6347.014834353151</v>
       </c>
       <c r="AE11">
-        <v>10225.07299152593</v>
+        <v>-1723.822070089501</v>
       </c>
       <c r="AF11">
-        <v>7706.260090258752</v>
+        <v>3454.704209384252</v>
       </c>
       <c r="AG11">
-        <v>1878.824864764929</v>
+        <v>1870.675945153846</v>
       </c>
       <c r="AH11">
-        <v>5848.922145185898</v>
+        <v>6136.361739698586</v>
       </c>
       <c r="AI11">
-        <v>10096.7769400159</v>
+        <v>3004.631227135381</v>
       </c>
       <c r="AJ11">
-        <v>7241.092896470421</v>
+        <v>15969.914537866</v>
       </c>
       <c r="AK11">
-        <v>9514.200487947573</v>
+        <v>10565.82640902071</v>
       </c>
       <c r="AL11">
-        <v>8311.061509389914</v>
+        <v>3927.130901968368</v>
       </c>
       <c r="AM11">
-        <v>8968.770161557575</v>
+        <v>12093.08611100737</v>
       </c>
       <c r="AN11">
-        <v>10927.30461294283</v>
+        <v>6515.612380677412</v>
       </c>
       <c r="AO11">
-        <v>6253.344340071782</v>
+        <v>1721.776634031648</v>
       </c>
       <c r="AP11">
-        <v>9152.435928333449</v>
+        <v>4057.054819930891</v>
       </c>
       <c r="AQ11">
-        <v>11499.60819879318</v>
+        <v>-914.4539074807236</v>
       </c>
       <c r="AR11">
-        <v>2335.03996760163</v>
+        <v>10209.25619941223</v>
       </c>
       <c r="AS11">
-        <v>12228.06842677884</v>
+        <v>-2770.474031071838</v>
       </c>
       <c r="AT11">
-        <v>4877.016468328822</v>
+        <v>5055.019127996511</v>
       </c>
       <c r="AU11">
-        <v>-858.9602796808541</v>
+        <v>2451.179063945979</v>
       </c>
       <c r="AV11">
-        <v>2331.612812899426</v>
+        <v>2027.859959599721</v>
       </c>
       <c r="AW11">
-        <v>2207.90028709749</v>
+        <v>-1013.415848600612</v>
       </c>
       <c r="AX11">
-        <v>2103.54764343033</v>
+        <v>-3198.412670190139</v>
       </c>
       <c r="AY11">
-        <v>4573.413319123701</v>
+        <v>-837.5016684156911</v>
       </c>
     </row>
     <row r="12" spans="1:51">
@@ -2106,154 +2106,154 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-2.026290834328857</v>
+        <v>-2.013426501522443</v>
       </c>
       <c r="C12">
-        <v>-2.025189144721001</v>
+        <v>-2.03101905923265</v>
       </c>
       <c r="D12">
-        <v>-2.01001425478279</v>
+        <v>-2.037850000867309</v>
       </c>
       <c r="E12">
-        <v>-2.025038259544519</v>
+        <v>-2.025591691265439</v>
       </c>
       <c r="F12">
-        <v>-2.019143021619934</v>
+        <v>-2.010797788493603</v>
       </c>
       <c r="G12">
-        <v>-2.02780243957072</v>
+        <v>-2.022186909249807</v>
       </c>
       <c r="H12">
-        <v>-2.022448623116825</v>
+        <v>-2.016694165810569</v>
       </c>
       <c r="I12">
-        <v>-2.015768955753923</v>
+        <v>-2.018663114317699</v>
       </c>
       <c r="J12">
-        <v>-2.021610949719961</v>
+        <v>-2.018581764720562</v>
       </c>
       <c r="K12">
-        <v>-2.02281747603353</v>
+        <v>-2.035325812107242</v>
       </c>
       <c r="L12">
-        <v>-2.028075981820188</v>
+        <v>-2.019501515862378</v>
       </c>
       <c r="M12">
-        <v>-2.033715305698978</v>
+        <v>-2.027549419919368</v>
       </c>
       <c r="N12">
-        <v>-2.022132235375131</v>
+        <v>-2.005029911699469</v>
       </c>
       <c r="O12">
-        <v>-2.012002852420093</v>
+        <v>-2.029440534959868</v>
       </c>
       <c r="P12">
-        <v>-2.012680250080126</v>
+        <v>-2.004093220330279</v>
       </c>
       <c r="Q12">
-        <v>-2.015002969588089</v>
+        <v>-2.024408153643561</v>
       </c>
       <c r="R12">
-        <v>-2.032699490381865</v>
+        <v>-2.021380798298662</v>
       </c>
       <c r="S12">
-        <v>-2.02162504657843</v>
+        <v>-2.030773320407209</v>
       </c>
       <c r="T12">
-        <v>-2.025086075987051</v>
+        <v>-2.017600443027268</v>
       </c>
       <c r="U12">
-        <v>-2.029343495560995</v>
+        <v>-2.012183803166998</v>
       </c>
       <c r="V12">
-        <v>-2.025786530953337</v>
+        <v>-2.031265104024153</v>
       </c>
       <c r="W12">
-        <v>-2.029309826685075</v>
+        <v>-2.009634988500969</v>
       </c>
       <c r="X12">
-        <v>-2.0269908338885</v>
+        <v>-2.010410987876007</v>
       </c>
       <c r="Y12">
-        <v>-2.015752592114275</v>
+        <v>-2.039539571862913</v>
       </c>
       <c r="Z12">
-        <v>-2.016723708988454</v>
+        <v>-2.015350237271995</v>
       </c>
       <c r="AA12">
-        <v>-2.024600683635957</v>
+        <v>-2.038135601293797</v>
       </c>
       <c r="AB12">
-        <v>-2.026284296250484</v>
+        <v>-2.021868400850013</v>
       </c>
       <c r="AC12">
-        <v>-2.01824928476415</v>
+        <v>-2.02759574153422</v>
       </c>
       <c r="AD12">
-        <v>-2.033714884277577</v>
+        <v>-2.01753849860972</v>
       </c>
       <c r="AE12">
-        <v>-2.020169121069081</v>
+        <v>-2.03297216449055</v>
       </c>
       <c r="AF12">
-        <v>-2.026049487823169</v>
+        <v>-2.008845416512783</v>
       </c>
       <c r="AG12">
-        <v>-2.011549668962097</v>
+        <v>-2.033054054415321</v>
       </c>
       <c r="AH12">
-        <v>-2.015200040081936</v>
+        <v>-2.026269312149773</v>
       </c>
       <c r="AI12">
-        <v>-2.016982877429011</v>
+        <v>-2.014338667401352</v>
       </c>
       <c r="AJ12">
-        <v>-2.036792578710692</v>
+        <v>-1.995633730526604</v>
       </c>
       <c r="AK12">
-        <v>-2.030401294942295</v>
+        <v>-2.032364832907807</v>
       </c>
       <c r="AL12">
-        <v>-2.018411365045464</v>
+        <v>-2.039956278867338</v>
       </c>
       <c r="AM12">
-        <v>-2.05745235859693</v>
+        <v>-2.026357999867824</v>
       </c>
       <c r="AN12">
-        <v>-2.026667723453789</v>
+        <v>-2.024042837279913</v>
       </c>
       <c r="AO12">
-        <v>-2.007167137765889</v>
+        <v>-2.008969685329907</v>
       </c>
       <c r="AP12">
-        <v>-2.018922052829877</v>
+        <v>-2.027773644362939</v>
       </c>
       <c r="AQ12">
-        <v>-2.047858658405931</v>
+        <v>-2.037328698566036</v>
       </c>
       <c r="AR12">
-        <v>-2.005514916383161</v>
+        <v>-2.011571559713692</v>
       </c>
       <c r="AS12">
-        <v>-2.022698699593456</v>
+        <v>-2.034850969118096</v>
       </c>
       <c r="AT12">
-        <v>-2.032432437764061</v>
+        <v>-2.023204542315401</v>
       </c>
       <c r="AU12">
-        <v>-2.017339076054855</v>
+        <v>-2.026245263482349</v>
       </c>
       <c r="AV12">
-        <v>-2.023697521118729</v>
+        <v>-2.028370221242534</v>
       </c>
       <c r="AW12">
-        <v>-2.028986521704077</v>
+        <v>-2.017507942685168</v>
       </c>
       <c r="AX12">
-        <v>-2.018340888362455</v>
+        <v>-2.019320042560471</v>
       </c>
       <c r="AY12">
-        <v>-2.016067144423084</v>
+        <v>-2.030613513529784</v>
       </c>
     </row>
     <row r="13" spans="1:51">
@@ -2261,154 +2261,154 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-1.396333124290374</v>
+        <v>-1.771423942177967</v>
       </c>
       <c r="C13">
-        <v>-1.423674456212344</v>
+        <v>-1.440045346956176</v>
       </c>
       <c r="D13">
-        <v>-1.450178028364054</v>
+        <v>-1.539092237572457</v>
       </c>
       <c r="E13">
-        <v>-1.911721853869344</v>
+        <v>-1.306441396723476</v>
       </c>
       <c r="F13">
-        <v>-1.421807983366675</v>
+        <v>-1.224243194068082</v>
       </c>
       <c r="G13">
-        <v>-1.389657506770762</v>
+        <v>-1.450114838022804</v>
       </c>
       <c r="H13">
-        <v>-1.489919537107047</v>
+        <v>-1.331913316021453</v>
       </c>
       <c r="I13">
-        <v>-1.356521511202212</v>
+        <v>-1.552879811530146</v>
       </c>
       <c r="J13">
-        <v>-1.682627121035804</v>
+        <v>-1.451412346451334</v>
       </c>
       <c r="K13">
-        <v>-1.390461558513473</v>
+        <v>-1.492106775336223</v>
       </c>
       <c r="L13">
-        <v>-1.360492239437758</v>
+        <v>-1.108000869254446</v>
       </c>
       <c r="M13">
-        <v>-1.587129502704177</v>
+        <v>-1.484845397317095</v>
       </c>
       <c r="N13">
-        <v>-1.37791078321948</v>
+        <v>-1.664576913296148</v>
       </c>
       <c r="O13">
-        <v>-1.381948688027399</v>
+        <v>-1.417998102330704</v>
       </c>
       <c r="P13">
-        <v>-1.728098292948007</v>
+        <v>-1.912216904259073</v>
       </c>
       <c r="Q13">
-        <v>-1.641024953369393</v>
+        <v>-1.507494949869328</v>
       </c>
       <c r="R13">
-        <v>-1.52473044411676</v>
+        <v>-1.37668216881115</v>
       </c>
       <c r="S13">
-        <v>-1.29479964402982</v>
+        <v>-1.288384888805694</v>
       </c>
       <c r="T13">
-        <v>-1.244161201603882</v>
+        <v>-1.462868728780158</v>
       </c>
       <c r="U13">
-        <v>-1.172336338829644</v>
+        <v>-1.548005423080448</v>
       </c>
       <c r="V13">
-        <v>-1.735680370399169</v>
+        <v>-1.769404275084966</v>
       </c>
       <c r="W13">
-        <v>-1.393587317420892</v>
+        <v>-1.511633697497628</v>
       </c>
       <c r="X13">
-        <v>-1.416787785921175</v>
+        <v>-1.367070913778327</v>
       </c>
       <c r="Y13">
-        <v>-1.308308434140618</v>
+        <v>-1.77328392706821</v>
       </c>
       <c r="Z13">
-        <v>-1.344952010327545</v>
+        <v>-1.24891890647489</v>
       </c>
       <c r="AA13">
-        <v>-1.120992466620449</v>
+        <v>-1.599822945348336</v>
       </c>
       <c r="AB13">
-        <v>-1.290669023969163</v>
+        <v>-1.695754824444097</v>
       </c>
       <c r="AC13">
-        <v>-1.315779000416074</v>
+        <v>-1.709657700804075</v>
       </c>
       <c r="AD13">
-        <v>-1.314554948709729</v>
+        <v>-1.384383388172944</v>
       </c>
       <c r="AE13">
-        <v>-1.5210209319546</v>
+        <v>-1.644319248016313</v>
       </c>
       <c r="AF13">
-        <v>-1.409088406223447</v>
+        <v>-1.465721500298384</v>
       </c>
       <c r="AG13">
-        <v>-1.503668159511091</v>
+        <v>-1.503394818428153</v>
       </c>
       <c r="AH13">
-        <v>-1.760669546997971</v>
+        <v>-1.493463873052643</v>
       </c>
       <c r="AI13">
-        <v>-1.923532581339035</v>
+        <v>-1.613221914043425</v>
       </c>
       <c r="AJ13">
-        <v>-1.96910273372245</v>
+        <v>-1.49977796847671</v>
       </c>
       <c r="AK13">
-        <v>-1.320251961739017</v>
+        <v>-1.72422519448448</v>
       </c>
       <c r="AL13">
-        <v>-1.577191189430991</v>
+        <v>-1.880023449415127</v>
       </c>
       <c r="AM13">
-        <v>-1.523977729629088</v>
+        <v>-1.557061977521996</v>
       </c>
       <c r="AN13">
-        <v>-1.67871183720188</v>
+        <v>-1.636432180959566</v>
       </c>
       <c r="AO13">
-        <v>-1.778681224262607</v>
+        <v>-1.628030439418614</v>
       </c>
       <c r="AP13">
-        <v>-1.631021780906165</v>
+        <v>-1.562529013425536</v>
       </c>
       <c r="AQ13">
-        <v>-1.433880714302585</v>
+        <v>-1.593750322920267</v>
       </c>
       <c r="AR13">
-        <v>-1.370989701235007</v>
+        <v>-1.561919894723504</v>
       </c>
       <c r="AS13">
-        <v>-1.559501587804924</v>
+        <v>-1.522500520113479</v>
       </c>
       <c r="AT13">
-        <v>-2.225620564058221</v>
+        <v>-1.552272593245381</v>
       </c>
       <c r="AU13">
-        <v>-1.82823292896206</v>
+        <v>-1.614451515092155</v>
       </c>
       <c r="AV13">
-        <v>-1.62829451635596</v>
+        <v>-1.855522181685785</v>
       </c>
       <c r="AW13">
-        <v>-1.665299259047106</v>
+        <v>-1.658610593505053</v>
       </c>
       <c r="AX13">
-        <v>-1.734313548483622</v>
+        <v>-1.539701422004415</v>
       </c>
       <c r="AY13">
-        <v>-1.759058624713834</v>
+        <v>-1.11847254915544</v>
       </c>
     </row>
     <row r="14" spans="1:51">
@@ -2416,154 +2416,154 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-1.328270176003408</v>
+        <v>-1.702959199942318</v>
       </c>
       <c r="C14">
-        <v>-1.355083805702873</v>
+        <v>-1.371931344537846</v>
       </c>
       <c r="D14">
-        <v>-1.381475242962548</v>
+        <v>-1.470302308986392</v>
       </c>
       <c r="E14">
-        <v>-1.842819338510777</v>
+        <v>-1.237937636288291</v>
       </c>
       <c r="F14">
-        <v>-1.353437426404755</v>
+        <v>-1.155418539668591</v>
       </c>
       <c r="G14">
-        <v>-1.320761254488607</v>
+        <v>-1.382675391095178</v>
       </c>
       <c r="H14">
-        <v>-1.420154675876578</v>
+        <v>-1.262699604583351</v>
       </c>
       <c r="I14">
-        <v>-1.288286151352994</v>
+        <v>-1.484196432289442</v>
       </c>
       <c r="J14">
-        <v>-1.61398325395089</v>
+        <v>-1.383213932581916</v>
       </c>
       <c r="K14">
-        <v>-1.323186040428473</v>
+        <v>-1.425422078526718</v>
       </c>
       <c r="L14">
-        <v>-1.291470832815384</v>
+        <v>-1.03965115093471</v>
       </c>
       <c r="M14">
-        <v>-1.519656836301875</v>
+        <v>-1.417835066790006</v>
       </c>
       <c r="N14">
-        <v>-1.309855726201401</v>
+        <v>-1.595574079132742</v>
       </c>
       <c r="O14">
-        <v>-1.313949430457274</v>
+        <v>-1.349596704635875</v>
       </c>
       <c r="P14">
-        <v>-1.659516765838922</v>
+        <v>-1.843641716736943</v>
       </c>
       <c r="Q14">
-        <v>-1.573056749495158</v>
+        <v>-1.438808419130338</v>
       </c>
       <c r="R14">
-        <v>-1.456801714206186</v>
+        <v>-1.307743832015239</v>
       </c>
       <c r="S14">
-        <v>-1.226423690652875</v>
+        <v>-1.219748460485899</v>
       </c>
       <c r="T14">
-        <v>-1.175200380588479</v>
+        <v>-1.3943276694775</v>
       </c>
       <c r="U14">
-        <v>-1.105523307556884</v>
+        <v>-1.479670447477838</v>
       </c>
       <c r="V14">
-        <v>-1.667507597971163</v>
+        <v>-1.7010278488507</v>
       </c>
       <c r="W14">
-        <v>-1.325723721586197</v>
+        <v>-1.443423273884859</v>
       </c>
       <c r="X14">
-        <v>-1.349055764685642</v>
+        <v>-1.299260855738417</v>
       </c>
       <c r="Y14">
-        <v>-1.241113976931257</v>
+        <v>-1.70440187088556</v>
       </c>
       <c r="Z14">
-        <v>-1.275615976498815</v>
+        <v>-1.180904042278218</v>
       </c>
       <c r="AA14">
-        <v>-1.053188902457846</v>
+        <v>-1.530469514860573</v>
       </c>
       <c r="AB14">
-        <v>-1.22306541454861</v>
+        <v>-1.627004465401006</v>
       </c>
       <c r="AC14">
-        <v>-1.247685959308145</v>
+        <v>-1.640913791747985</v>
       </c>
       <c r="AD14">
-        <v>-1.24667891767825</v>
+        <v>-1.316373700128935</v>
       </c>
       <c r="AE14">
-        <v>-1.452705790516117</v>
+        <v>-1.575322789874731</v>
       </c>
       <c r="AF14">
-        <v>-1.340551489235279</v>
+        <v>-1.397154151130773</v>
       </c>
       <c r="AG14">
-        <v>-1.435775436565655</v>
+        <v>-1.435087420105764</v>
       </c>
       <c r="AH14">
-        <v>-1.692171918085267</v>
+        <v>-1.425269331157782</v>
       </c>
       <c r="AI14">
-        <v>-1.855315853029778</v>
+        <v>-1.545179354583872</v>
       </c>
       <c r="AJ14">
-        <v>-1.901632445229739</v>
+        <v>-1.431288551740486</v>
       </c>
       <c r="AK14">
-        <v>-1.252244025278697</v>
+        <v>-1.65520028155208</v>
       </c>
       <c r="AL14">
-        <v>-1.509112147868796</v>
+        <v>-1.811450895538746</v>
       </c>
       <c r="AM14">
-        <v>-1.454834773857673</v>
+        <v>-1.488592564699918</v>
       </c>
       <c r="AN14">
-        <v>-1.609711411930271</v>
+        <v>-1.568387639949927</v>
       </c>
       <c r="AO14">
-        <v>-1.710996752230063</v>
+        <v>-1.559246550563099</v>
       </c>
       <c r="AP14">
-        <v>-1.563312177862132</v>
+        <v>-1.49377676127536</v>
       </c>
       <c r="AQ14">
-        <v>-1.365420812649604</v>
+        <v>-1.524372941965245</v>
       </c>
       <c r="AR14">
-        <v>-1.302958581492944</v>
+        <v>-1.493364068572028</v>
       </c>
       <c r="AS14">
-        <v>-1.491185038682446</v>
+        <v>-1.453975678140758</v>
       </c>
       <c r="AT14">
-        <v>-2.157623504773726</v>
+        <v>-1.484066011228268</v>
       </c>
       <c r="AU14">
-        <v>-1.76051183722878</v>
+        <v>-1.545963490819878</v>
       </c>
       <c r="AV14">
-        <v>-1.560330617410497</v>
+        <v>-1.787226695589803</v>
       </c>
       <c r="AW14">
-        <v>-1.596318505482493</v>
+        <v>-1.590042234034576</v>
       </c>
       <c r="AX14">
-        <v>-1.666827959950984</v>
+        <v>-1.470362083239082</v>
       </c>
       <c r="AY14">
-        <v>-1.691035349921379</v>
+        <v>-1.049504109546029</v>
       </c>
     </row>
     <row r="15" spans="1:51">
@@ -2571,154 +2571,154 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2.024461021132106</v>
+        <v>1.67061671800866</v>
       </c>
       <c r="C15">
-        <v>2.027989226927419</v>
+        <v>1.981496587455223</v>
       </c>
       <c r="D15">
-        <v>2.009267829725786</v>
+        <v>1.926421888479269</v>
       </c>
       <c r="E15">
-        <v>1.563627274738627</v>
+        <v>2.143946622531465</v>
       </c>
       <c r="F15">
-        <v>2.018125722779845</v>
+        <v>2.239599088073508</v>
       </c>
       <c r="G15">
-        <v>2.076603521796377</v>
+        <v>1.937200164969295</v>
       </c>
       <c r="H15">
-        <v>2.028917655501235</v>
+        <v>2.162662003359799</v>
       </c>
       <c r="I15">
-        <v>2.073707650104364</v>
+        <v>1.901989669506443</v>
       </c>
       <c r="J15">
-        <v>1.769958697385352</v>
+        <v>1.97703459304327</v>
       </c>
       <c r="K15">
-        <v>1.982244230133454</v>
+        <v>1.854731525150013</v>
       </c>
       <c r="L15">
-        <v>2.118225689410447</v>
+        <v>2.33738895816895</v>
       </c>
       <c r="M15">
-        <v>1.806488147409391</v>
+        <v>1.878009154671685</v>
       </c>
       <c r="N15">
-        <v>2.042473280940046</v>
+        <v>1.810558640309455</v>
       </c>
       <c r="O15">
-        <v>2.035700009064279</v>
+        <v>2.02450682819446</v>
       </c>
       <c r="P15">
-        <v>1.725751825233912</v>
+        <v>1.536694204893567</v>
       </c>
       <c r="Q15">
-        <v>1.777898069620401</v>
+        <v>1.951935396203577</v>
       </c>
       <c r="R15">
-        <v>1.893694932810616</v>
+        <v>2.094172712158957</v>
       </c>
       <c r="S15">
-        <v>2.144658842970185</v>
+        <v>2.167580128779809</v>
       </c>
       <c r="T15">
-        <v>2.221573329147069</v>
+        <v>1.986528552434538</v>
       </c>
       <c r="U15">
-        <v>2.181152521116549</v>
+        <v>1.889460361674687</v>
       </c>
       <c r="V15">
-        <v>1.695572386217157</v>
+        <v>1.672483550050637</v>
       </c>
       <c r="W15">
-        <v>2.01337696064836</v>
+        <v>1.923497694241063</v>
       </c>
       <c r="X15">
-        <v>1.983521930525781</v>
+        <v>2.038175526015882</v>
       </c>
       <c r="Y15">
-        <v>2.063406365666553</v>
+        <v>1.697022268398652</v>
       </c>
       <c r="Z15">
-        <v>2.155250247212384</v>
+        <v>2.169251899770032</v>
       </c>
       <c r="AA15">
-        <v>2.287498960474565</v>
+        <v>1.895151761934565</v>
       </c>
       <c r="AB15">
-        <v>2.107509998899689</v>
+        <v>1.772034648177312</v>
       </c>
       <c r="AC15">
-        <v>2.108381682251463</v>
+        <v>1.753012828676566</v>
       </c>
       <c r="AD15">
-        <v>2.098372487673173</v>
+        <v>2.033835965121916</v>
       </c>
       <c r="AE15">
-        <v>1.914593315871247</v>
+        <v>1.834083711260518</v>
       </c>
       <c r="AF15">
-        <v>2.040110949524259</v>
+        <v>1.983459579390861</v>
       </c>
       <c r="AG15">
-        <v>1.909385658241809</v>
+        <v>1.933906038800159</v>
       </c>
       <c r="AH15">
-        <v>1.684150155587845</v>
+        <v>1.936181596873794</v>
       </c>
       <c r="AI15">
-        <v>1.506049372299198</v>
+        <v>1.809394606369615</v>
       </c>
       <c r="AJ15">
-        <v>1.425126650716784</v>
+        <v>1.953417056592791</v>
       </c>
       <c r="AK15">
-        <v>2.100786999594792</v>
+        <v>1.756746499939347</v>
       </c>
       <c r="AL15">
-        <v>1.84624947491874</v>
+        <v>1.571651943792101</v>
       </c>
       <c r="AM15">
-        <v>1.956259161616245</v>
+        <v>1.889156608270731</v>
       </c>
       <c r="AN15">
-        <v>1.800267325648208</v>
+        <v>1.783150245861179</v>
       </c>
       <c r="AO15">
-        <v>1.624525039154407</v>
+        <v>1.840313490329155</v>
       </c>
       <c r="AP15">
-        <v>1.769888132717992</v>
+        <v>1.898133857557604</v>
       </c>
       <c r="AQ15">
-        <v>2.012998030336639</v>
+        <v>1.91122043978241</v>
       </c>
       <c r="AR15">
-        <v>2.046220012534332</v>
+        <v>1.891569449061252</v>
       </c>
       <c r="AS15">
-        <v>1.87906469055883</v>
+        <v>1.928007134650672</v>
       </c>
       <c r="AT15">
-        <v>1.192883208679644</v>
+        <v>1.876430615808631</v>
       </c>
       <c r="AU15">
-        <v>1.576472714245772</v>
+        <v>1.833076959007617</v>
       </c>
       <c r="AV15">
-        <v>1.787560208580165</v>
+        <v>1.580356357997296</v>
       </c>
       <c r="AW15">
-        <v>1.809904139791006</v>
+        <v>1.78651688157407</v>
       </c>
       <c r="AX15">
-        <v>1.656142893575974</v>
+        <v>1.952384875032164</v>
       </c>
       <c r="AY15">
-        <v>1.660576110949087</v>
+        <v>2.355878802958161</v>
       </c>
     </row>
     <row r="16" spans="1:51">

</xml_diff>

<commit_message>
modified:   MonteCarlo_Sim.py 	modified:   Outputs/MonteCarlo_sim_inputs.xlsx 	modified:   Outputs/MonteCarlo_sim_outputs.xlsx 	modified:   Outputs/MonteCarlo_sim_wind.xlsx 	modified:   Tools.py
</commit_message>
<xml_diff>
--- a/Outputs/MonteCarlo_sim_outputs.xlsx
+++ b/Outputs/MonteCarlo_sim_outputs.xlsx
@@ -412,10 +412,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.3932893430561388</v>
+        <v>0.3968591891046255</v>
       </c>
       <c r="C2">
-        <v>0.392707584027212</v>
+        <v>0.3932745487300524</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -423,10 +423,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>46.49187048396569</v>
+        <v>46.08271915157921</v>
       </c>
       <c r="C3">
-        <v>46.58285920086178</v>
+        <v>46.46138267323168</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -434,10 +434,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>749.9267663892135</v>
+        <v>773.0656828242987</v>
       </c>
       <c r="C4">
-        <v>779.6498010712982</v>
+        <v>769.8464956551795</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -445,10 +445,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>69.30000297728797</v>
+        <v>72.76409810354545</v>
       </c>
       <c r="C5">
-        <v>73.20397039299054</v>
+        <v>68.55733984940724</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -456,10 +456,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>23825.80346679897</v>
+        <v>25935.8031076495</v>
       </c>
       <c r="C6">
-        <v>26321.73999868403</v>
+        <v>23758.85461543648</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -467,10 +467,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>800.55176196153</v>
+        <v>953.4433762394547</v>
       </c>
       <c r="C7">
-        <v>1629.884265411335</v>
+        <v>1313.62912996436</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -478,10 +478,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-3323.033283483964</v>
+        <v>-2333.170494236158</v>
       </c>
       <c r="C8">
-        <v>-134.8684947084942</v>
+        <v>98.07242789251477</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -489,10 +489,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>573.5950408142635</v>
+        <v>582.295169670233</v>
       </c>
       <c r="C9">
-        <v>585.9698573663768</v>
+        <v>567.2022375458338</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -500,10 +500,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3233.801199996195</v>
+        <v>3360.526318588844</v>
       </c>
       <c r="C10">
-        <v>5789.876948055387</v>
+        <v>4179.677015473537</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -511,10 +511,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1200.982765475774</v>
+        <v>-1455.95198368039</v>
       </c>
       <c r="C11">
-        <v>-377.4169906115071</v>
+        <v>-403.9338758972591</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -522,10 +522,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-8.476519280220081</v>
+        <v>-8.438350680131276</v>
       </c>
       <c r="C12">
-        <v>-8.447478717021379</v>
+        <v>-8.406545210008485</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -533,10 +533,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-4.084752035566997</v>
+        <v>-4.345022509496995</v>
       </c>
       <c r="C13">
-        <v>-4.339545630489408</v>
+        <v>-4.493072200383833</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -544,10 +544,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-4.025304721551356</v>
+        <v>-4.283884224258766</v>
       </c>
       <c r="C14">
-        <v>-4.28022145767423</v>
+        <v>-4.433297209417767</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -555,10 +555,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.7533606021254471</v>
+        <v>-0.9031443591398607</v>
       </c>
       <c r="C15">
-        <v>-1.019443756518071</v>
+        <v>-1.141731157285696</v>
       </c>
     </row>
     <row r="16" spans="1:3">

</xml_diff>